<commit_message>
2 months of progress
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Telic\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7CEB4D2-519C-4FE9-8678-CB77979C4C8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD7A6FDE-A45A-4C1B-9196-9CF92C097A19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25005" yWindow="945" windowWidth="32595" windowHeight="14070" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="17175" yWindow="345" windowWidth="25995" windowHeight="14070" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -50,10 +50,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -406,10 +412,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:D76"/>
+  <dimension ref="A1:D114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F73" sqref="F73"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F115" sqref="F115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +948,7 @@
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
-        <v>44816</v>
+        <v>44846</v>
       </c>
       <c r="B59" s="5">
         <v>1</v>
@@ -952,7 +958,7 @@
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
-        <v>44817</v>
+        <v>44847</v>
       </c>
       <c r="B60" s="5">
         <v>1</v>
@@ -962,7 +968,7 @@
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
-        <v>44818</v>
+        <v>44848</v>
       </c>
       <c r="B61" s="5">
         <v>3</v>
@@ -972,7 +978,7 @@
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="B62" s="5">
         <v>4</v>
@@ -982,7 +988,7 @@
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
-        <v>44820</v>
+        <v>44850</v>
       </c>
       <c r="B63" s="5">
         <v>4</v>
@@ -995,7 +1001,7 @@
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
-        <v>44821</v>
+        <v>44851</v>
       </c>
       <c r="B65" s="5">
         <v>1</v>
@@ -1005,7 +1011,7 @@
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
-        <v>44822</v>
+        <v>44852</v>
       </c>
       <c r="B66" s="5">
         <v>0</v>
@@ -1015,7 +1021,7 @@
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
-        <v>44823</v>
+        <v>44853</v>
       </c>
       <c r="B67" s="5">
         <v>0</v>
@@ -1025,7 +1031,7 @@
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
-        <v>44824</v>
+        <v>44854</v>
       </c>
       <c r="B68" s="5">
         <v>0</v>
@@ -1035,7 +1041,7 @@
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
-        <v>44825</v>
+        <v>44855</v>
       </c>
       <c r="B69" s="5">
         <v>4</v>
@@ -1045,35 +1051,412 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
-        <v>44826</v>
+        <v>44856</v>
       </c>
       <c r="B70" s="5">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
-        <v>44827</v>
+        <v>44857</v>
       </c>
       <c r="B71" s="5">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="C71" s="5"/>
-      <c r="D71" s="5"/>
+      <c r="D71" s="5">
+        <f>SUM(B65:B71) + 42</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4">
+        <v>44858</v>
+      </c>
+      <c r="B73" s="5">
+        <v>0</v>
+      </c>
+      <c r="C73" s="5"/>
+      <c r="D73" s="5"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="4">
+        <v>44859</v>
+      </c>
+      <c r="B74" s="5">
+        <v>2</v>
+      </c>
+      <c r="C74" s="5"/>
+      <c r="D74" s="5"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="4">
+        <v>44860</v>
+      </c>
+      <c r="B75" s="5">
+        <v>8</v>
+      </c>
+      <c r="C75" s="5"/>
+      <c r="D75" s="5"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="4">
+        <v>44861</v>
+      </c>
       <c r="B76" s="5">
-        <f>SUM(B2:B71)</f>
-        <v>226</v>
-      </c>
-      <c r="C76">
-        <f>B76/7</f>
-        <v>32.285714285714285</v>
+        <v>11</v>
+      </c>
+      <c r="C76" s="5"/>
+      <c r="D76" s="5"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="4">
+        <v>44862</v>
+      </c>
+      <c r="B77" s="5">
+        <v>7</v>
+      </c>
+      <c r="C77" s="5"/>
+      <c r="D77" s="5"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="4">
+        <v>44863</v>
+      </c>
+      <c r="B78" s="5">
+        <v>11</v>
+      </c>
+      <c r="C78" s="5"/>
+      <c r="D78" s="5"/>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="4">
+        <v>44864</v>
+      </c>
+      <c r="B79" s="5">
+        <v>6</v>
+      </c>
+      <c r="C79" s="5"/>
+      <c r="D79" s="5">
+        <f>SUM(B73:B79) + 16</f>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="4">
+        <v>44865</v>
+      </c>
+      <c r="B81" s="5">
+        <v>8</v>
+      </c>
+      <c r="C81" s="5"/>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="4">
+        <v>44866</v>
+      </c>
+      <c r="B82" s="5">
+        <v>4</v>
+      </c>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="4">
+        <v>44867</v>
+      </c>
+      <c r="B83" s="5">
+        <v>7</v>
+      </c>
+      <c r="C83" s="5"/>
+      <c r="D83" s="5"/>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="4">
+        <v>44868</v>
+      </c>
+      <c r="B84" s="5">
+        <v>5</v>
+      </c>
+      <c r="C84" s="5"/>
+      <c r="D84" s="5"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="4">
+        <v>44869</v>
+      </c>
+      <c r="B85" s="5">
+        <v>4</v>
+      </c>
+      <c r="C85" s="5"/>
+      <c r="D85" s="5"/>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="4">
+        <v>44870</v>
+      </c>
+      <c r="B86" s="5">
+        <v>6</v>
+      </c>
+      <c r="C86" s="5"/>
+      <c r="D86" s="5"/>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="4">
+        <v>44871</v>
+      </c>
+      <c r="B87" s="5">
+        <v>3</v>
+      </c>
+      <c r="C87" s="5"/>
+      <c r="D87" s="5"/>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="4">
+        <v>44871</v>
+      </c>
+      <c r="B89" s="5">
+        <v>2</v>
+      </c>
+      <c r="C89" s="5"/>
+      <c r="D89" s="5"/>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="4">
+        <v>44872</v>
+      </c>
+      <c r="B90" s="5">
+        <v>4</v>
+      </c>
+      <c r="C90" s="5"/>
+      <c r="D90" s="5"/>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="4">
+        <v>44873</v>
+      </c>
+      <c r="B91" s="5">
+        <v>0</v>
+      </c>
+      <c r="C91" s="5"/>
+      <c r="D91" s="5"/>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="4">
+        <v>44874</v>
+      </c>
+      <c r="B92" s="5">
+        <v>0</v>
+      </c>
+      <c r="C92" s="5"/>
+      <c r="D92" s="5"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" s="4">
+        <v>44875</v>
+      </c>
+      <c r="B93" s="5">
+        <v>0</v>
+      </c>
+      <c r="C93" s="5"/>
+      <c r="D93" s="5"/>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" s="4">
+        <v>44876</v>
+      </c>
+      <c r="B94" s="5">
+        <v>2</v>
+      </c>
+      <c r="C94" s="5"/>
+      <c r="D94" s="5"/>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="4">
+        <v>44877</v>
+      </c>
+      <c r="B95" s="5">
+        <v>0</v>
+      </c>
+      <c r="C95" s="5"/>
+      <c r="D95" s="5"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="4">
+        <v>44878</v>
+      </c>
+      <c r="B96" s="5"/>
+      <c r="C96" s="5"/>
+      <c r="D96" s="5"/>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="4">
+        <v>44879</v>
+      </c>
+      <c r="B98" s="5">
+        <v>2</v>
+      </c>
+      <c r="C98" s="5"/>
+      <c r="D98" s="5"/>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="4">
+        <v>44880</v>
+      </c>
+      <c r="B99" s="5">
+        <v>8</v>
+      </c>
+      <c r="C99" s="5"/>
+      <c r="D99" s="5"/>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="4">
+        <v>44881</v>
+      </c>
+      <c r="B100" s="5">
+        <v>4</v>
+      </c>
+      <c r="C100" s="5"/>
+      <c r="D100" s="5"/>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A101" s="4">
+        <v>44882</v>
+      </c>
+      <c r="B101" s="5">
+        <v>5</v>
+      </c>
+      <c r="C101" s="5"/>
+      <c r="D101" s="5">
+        <f>B101+10</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A102" s="4">
+        <v>44883</v>
+      </c>
+      <c r="B102" s="5">
+        <v>7</v>
+      </c>
+      <c r="C102" s="5"/>
+      <c r="D102" s="5">
+        <f>B102+6</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A103" s="4">
+        <v>44884</v>
+      </c>
+      <c r="B103" s="5">
+        <v>8</v>
+      </c>
+      <c r="C103" s="5"/>
+      <c r="D103" s="5"/>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104" s="4">
+        <v>44885</v>
+      </c>
+      <c r="B104" s="5">
+        <v>4</v>
+      </c>
+      <c r="C104" s="5"/>
+      <c r="D104" s="5">
+        <f>SUM(B98:B104) + 42</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106" s="4">
+        <v>44886</v>
+      </c>
+      <c r="B106" s="5">
+        <v>5</v>
+      </c>
+      <c r="C106" s="5"/>
+      <c r="D106" s="5"/>
+    </row>
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A107" s="4">
+        <v>44887</v>
+      </c>
+      <c r="B107" s="5">
+        <v>0</v>
+      </c>
+      <c r="C107" s="5"/>
+      <c r="D107" s="5"/>
+    </row>
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A108" s="4">
+        <v>44888</v>
+      </c>
+      <c r="B108" s="5">
+        <v>5</v>
+      </c>
+      <c r="C108" s="5"/>
+      <c r="D108" s="5"/>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109" s="4">
+        <v>44889</v>
+      </c>
+      <c r="B109" s="5">
+        <v>0</v>
+      </c>
+      <c r="C109" s="5"/>
+      <c r="D109" s="5"/>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" s="4">
+        <v>44890</v>
+      </c>
+      <c r="B110" s="5">
+        <v>5</v>
+      </c>
+      <c r="C110" s="5"/>
+      <c r="D110" s="5"/>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111" s="4">
+        <v>44891</v>
+      </c>
+      <c r="B111" s="5">
+        <v>12</v>
+      </c>
+      <c r="C111" s="5"/>
+      <c r="D111" s="5"/>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112" s="4">
+        <v>44892</v>
+      </c>
+      <c r="B112" s="5">
+        <v>10</v>
+      </c>
+      <c r="C112" s="5"/>
+      <c r="D112" s="5">
+        <f>SUM(B106:B112) + 42</f>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B114" s="5">
+        <f>SUM(B2:B112)</f>
+        <v>411</v>
+      </c>
+      <c r="C114">
+        <f>B114/12</f>
+        <v>34.25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Added NXP i.MX8 Project, Added Sensor Methods
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87140497-9C2E-4570-A36F-D67DE415177D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8370A8FA-1066-4A68-8D7F-413D0C823B1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19290" yWindow="825" windowWidth="27180" windowHeight="14070" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="27420" yWindow="2100" windowWidth="21060" windowHeight="13890" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -413,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:D195"/>
+  <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A181" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E190" sqref="E190"/>
+    <sheetView tabSelected="1" topLeftCell="A219" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H201" sqref="H201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2124,7 +2124,7 @@
         <v>44973</v>
       </c>
       <c r="B189" s="6">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
@@ -2134,7 +2134,7 @@
         <v>44974</v>
       </c>
       <c r="B190" s="6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
@@ -2144,23 +2144,341 @@
         <v>44975</v>
       </c>
       <c r="B191" s="6">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
     </row>
-    <row r="195" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A192" s="4">
+        <v>44976</v>
+      </c>
+      <c r="B192" s="6">
+        <v>5</v>
+      </c>
+      <c r="C192" s="4"/>
+      <c r="D192" s="4"/>
+    </row>
+    <row r="194" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A194" s="4">
+        <v>44977</v>
+      </c>
+      <c r="B194" s="5">
+        <v>1</v>
+      </c>
+      <c r="C194" s="4"/>
+      <c r="D194" s="4"/>
+    </row>
+    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A195" s="4">
+        <v>44978</v>
+      </c>
       <c r="B195" s="5">
-        <f>SUM(B2:B191)</f>
-        <v>790</v>
-      </c>
-      <c r="C195">
-        <f>B195/21</f>
-        <v>37.61904761904762</v>
-      </c>
-      <c r="D195">
-        <f>21*7</f>
-        <v>147</v>
+        <v>5</v>
+      </c>
+      <c r="C195" s="4"/>
+      <c r="D195" s="4"/>
+    </row>
+    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A196" s="4">
+        <v>44979</v>
+      </c>
+      <c r="B196" s="5">
+        <v>2</v>
+      </c>
+      <c r="C196" s="4"/>
+      <c r="D196" s="4"/>
+    </row>
+    <row r="197" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A197" s="4">
+        <v>44980</v>
+      </c>
+      <c r="B197" s="5">
+        <v>5</v>
+      </c>
+      <c r="C197" s="4"/>
+      <c r="D197" s="4"/>
+    </row>
+    <row r="198" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A198" s="4">
+        <v>44981</v>
+      </c>
+      <c r="B198" s="5">
+        <v>3</v>
+      </c>
+      <c r="C198" s="4"/>
+      <c r="D198" s="4"/>
+    </row>
+    <row r="199" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A199" s="4">
+        <v>44982</v>
+      </c>
+      <c r="B199" s="5">
+        <v>10</v>
+      </c>
+      <c r="C199" s="4"/>
+      <c r="D199" s="4"/>
+    </row>
+    <row r="200" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A200" s="4">
+        <v>44983</v>
+      </c>
+      <c r="B200" s="5">
+        <v>5</v>
+      </c>
+      <c r="C200" s="4"/>
+      <c r="D200" s="4"/>
+    </row>
+    <row r="202" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A202" s="4">
+        <v>44984</v>
+      </c>
+      <c r="B202" s="5">
+        <v>3</v>
+      </c>
+      <c r="C202" s="5"/>
+      <c r="D202" s="5"/>
+    </row>
+    <row r="203" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A203" s="4">
+        <v>44985</v>
+      </c>
+      <c r="B203" s="5">
+        <v>2</v>
+      </c>
+      <c r="C203" s="5"/>
+      <c r="D203" s="5"/>
+    </row>
+    <row r="204" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A204" s="4">
+        <v>44986</v>
+      </c>
+      <c r="B204" s="5">
+        <v>2</v>
+      </c>
+      <c r="C204" s="5"/>
+      <c r="D204" s="5"/>
+    </row>
+    <row r="205" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A205" s="4">
+        <v>44987</v>
+      </c>
+      <c r="B205" s="5">
+        <v>3</v>
+      </c>
+      <c r="C205" s="5"/>
+      <c r="D205" s="5"/>
+    </row>
+    <row r="206" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A206" s="4">
+        <v>44988</v>
+      </c>
+      <c r="B206" s="5">
+        <v>3</v>
+      </c>
+      <c r="C206" s="5"/>
+      <c r="D206" s="5"/>
+    </row>
+    <row r="207" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A207" s="4">
+        <v>44989</v>
+      </c>
+      <c r="B207" s="5">
+        <v>9</v>
+      </c>
+      <c r="C207" s="5"/>
+      <c r="D207" s="5"/>
+    </row>
+    <row r="208" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A208" s="4">
+        <v>44990</v>
+      </c>
+      <c r="B208" s="5">
+        <v>7</v>
+      </c>
+      <c r="C208" s="5"/>
+      <c r="D208" s="5"/>
+    </row>
+    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A210" s="4">
+        <v>44991</v>
+      </c>
+      <c r="B210" s="5"/>
+      <c r="C210" s="5"/>
+      <c r="D210" s="5"/>
+    </row>
+    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A211" s="4">
+        <v>44992</v>
+      </c>
+      <c r="B211" s="5"/>
+      <c r="C211" s="5"/>
+      <c r="D211" s="5"/>
+    </row>
+    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A212" s="4">
+        <v>44993</v>
+      </c>
+      <c r="B212" s="5"/>
+      <c r="C212" s="5"/>
+      <c r="D212" s="5"/>
+    </row>
+    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A213" s="4">
+        <v>44994</v>
+      </c>
+      <c r="B213" s="5"/>
+      <c r="C213" s="5"/>
+      <c r="D213" s="5"/>
+    </row>
+    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A214" s="4">
+        <v>44995</v>
+      </c>
+      <c r="B214" s="5"/>
+      <c r="C214" s="5"/>
+      <c r="D214" s="5"/>
+    </row>
+    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A215" s="4">
+        <v>44996</v>
+      </c>
+      <c r="B215" s="5"/>
+      <c r="C215" s="5"/>
+      <c r="D215" s="5"/>
+    </row>
+    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A216" s="4">
+        <v>44997</v>
+      </c>
+      <c r="B216" s="5"/>
+      <c r="C216" s="5"/>
+      <c r="D216" s="5"/>
+    </row>
+    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A218" s="4">
+        <v>44998</v>
+      </c>
+      <c r="B218" s="5"/>
+      <c r="C218" s="5"/>
+      <c r="D218" s="5"/>
+    </row>
+    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A219" s="4">
+        <v>44999</v>
+      </c>
+      <c r="B219" s="5"/>
+      <c r="C219" s="5"/>
+      <c r="D219" s="5"/>
+    </row>
+    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A220" s="4">
+        <v>45000</v>
+      </c>
+      <c r="B220" s="5"/>
+      <c r="C220" s="5"/>
+      <c r="D220" s="5"/>
+    </row>
+    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A221" s="4">
+        <v>45001</v>
+      </c>
+      <c r="B221" s="5"/>
+      <c r="C221" s="5"/>
+      <c r="D221" s="5"/>
+    </row>
+    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A222" s="4">
+        <v>45002</v>
+      </c>
+      <c r="B222" s="5"/>
+      <c r="C222" s="5"/>
+      <c r="D222" s="5"/>
+    </row>
+    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A223" s="4">
+        <v>45003</v>
+      </c>
+      <c r="B223" s="5"/>
+      <c r="C223" s="5"/>
+      <c r="D223" s="5"/>
+    </row>
+    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A224" s="4">
+        <v>45004</v>
+      </c>
+      <c r="B224" s="5"/>
+      <c r="C224" s="5"/>
+      <c r="D224" s="5"/>
+    </row>
+    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A226" s="4">
+        <v>45005</v>
+      </c>
+      <c r="B226" s="5"/>
+      <c r="C226" s="5"/>
+      <c r="D226" s="5"/>
+    </row>
+    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A227" s="4">
+        <v>45006</v>
+      </c>
+      <c r="B227" s="5"/>
+      <c r="C227" s="5"/>
+      <c r="D227" s="5"/>
+    </row>
+    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A228" s="4">
+        <v>45007</v>
+      </c>
+      <c r="B228" s="5"/>
+      <c r="C228" s="5"/>
+      <c r="D228" s="5"/>
+    </row>
+    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A229" s="4">
+        <v>45008</v>
+      </c>
+      <c r="B229" s="5"/>
+      <c r="C229" s="5"/>
+      <c r="D229" s="5"/>
+    </row>
+    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A230" s="4">
+        <v>45009</v>
+      </c>
+      <c r="B230" s="5"/>
+      <c r="C230" s="5"/>
+      <c r="D230" s="5"/>
+    </row>
+    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A231" s="4">
+        <v>45010</v>
+      </c>
+      <c r="B231" s="5"/>
+      <c r="C231" s="5"/>
+      <c r="D231" s="5"/>
+    </row>
+    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A232" s="4">
+        <v>45011</v>
+      </c>
+      <c r="B232" s="5"/>
+      <c r="C232" s="5"/>
+      <c r="D232" s="5"/>
+    </row>
+    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B234" s="5">
+        <f>SUM(B2:B232)</f>
+        <v>881</v>
+      </c>
+      <c r="C234">
+        <f>B234/23</f>
+        <v>38.304347826086953</v>
+      </c>
+      <c r="D234">
+        <f>23*7</f>
+        <v>161</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added esp32 sensor code / working on AD8232
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0227C1D5-05DA-4901-B6B9-6C7FD8176380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B683E7CA-2E81-48AB-B2FE-AD8165AA6EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="27420" yWindow="2100" windowWidth="21060" windowHeight="13890" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="20115" yWindow="1560" windowWidth="21060" windowHeight="13890" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -91,14 +91,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -405,7 +402,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -415,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
   <dimension ref="A1:D234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A208" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D226" sqref="D226"/>
+    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G228" sqref="G228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -496,74 +493,74 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="A9" s="2">
         <v>44801</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>2</v>
       </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+      <c r="A10" s="2">
         <v>44802</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>4</v>
       </c>
-      <c r="C10" s="5"/>
-      <c r="D10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="A11" s="2">
         <v>44803</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>2</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="A12" s="2">
         <v>44805</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="A13" s="2">
         <v>44806</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>4</v>
       </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="A14" s="2">
         <v>44807</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>4</v>
       </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
+      <c r="A15" s="2">
         <v>44808</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>15</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5">
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
         <f>SUM(B9:B15)</f>
         <v>34</v>
       </c>
@@ -572,1939 +569,1954 @@
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="4">
+      <c r="A17" s="2">
         <v>44809</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>8</v>
       </c>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
+      <c r="A18" s="2">
         <v>44810</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>10</v>
       </c>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
+      <c r="A19" s="2">
         <v>44811</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="3">
         <v>12</v>
       </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
+      <c r="A20" s="2">
         <v>44812</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="A21" s="2">
         <v>44813</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="4">
+      <c r="A22" s="2">
         <v>44814</v>
       </c>
-      <c r="B22" s="5">
+      <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
+      <c r="A23" s="2">
         <v>44815</v>
       </c>
-      <c r="B23" s="5">
-        <v>0</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5">
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
         <f>SUM(B17:B23)</f>
         <v>39</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="4">
+      <c r="A25" s="2">
         <v>44816</v>
       </c>
-      <c r="B25" s="5">
-        <v>0</v>
-      </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="4">
+      <c r="A26" s="2">
         <v>44817</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="3">
         <v>7</v>
       </c>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="A27" s="2">
         <v>44818</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="3">
         <v>6</v>
       </c>
-      <c r="C27" s="5"/>
-      <c r="D27" s="5"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="A28" s="2">
         <v>44819</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="3">
         <v>3</v>
       </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="5"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="A29" s="2">
         <v>44820</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="3">
         <v>2</v>
       </c>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>44821</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="3">
         <v>9</v>
       </c>
-      <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <v>44822</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="3">
         <v>11</v>
       </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <v>44823</v>
       </c>
-      <c r="B33" s="5">
-        <v>0</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="2">
         <v>44824</v>
       </c>
-      <c r="B34" s="5">
-        <v>0</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <v>44825</v>
       </c>
-      <c r="B35" s="5">
+      <c r="B35" s="3">
         <v>2</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <v>44826</v>
       </c>
-      <c r="B36" s="5">
-        <v>0</v>
-      </c>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="2">
         <v>44827</v>
       </c>
-      <c r="B37" s="5">
-        <v>0</v>
-      </c>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <v>44828</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="3">
         <v>3</v>
       </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="2">
         <v>44829</v>
       </c>
-      <c r="B39" s="5">
-        <v>0</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3"/>
+      <c r="D39" s="3"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41" s="2">
         <v>44830</v>
       </c>
-      <c r="B41" s="5">
+      <c r="B41" s="3">
         <v>1</v>
       </c>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="C41" s="3"/>
+      <c r="D41" s="3"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="2">
         <v>44831</v>
       </c>
-      <c r="B42" s="5">
+      <c r="B42" s="3">
         <v>1</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="C42" s="3"/>
+      <c r="D42" s="3"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="2">
         <v>44832</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="3">
         <v>1</v>
       </c>
-      <c r="C43" s="5"/>
-      <c r="D43" s="5"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44" s="2">
         <v>44833</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="3">
         <v>1</v>
       </c>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45" s="2">
         <v>44834</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="3">
         <v>2</v>
       </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46" s="2">
         <v>44835</v>
       </c>
-      <c r="B46" s="5">
+      <c r="B46" s="3">
         <v>1</v>
       </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
+      <c r="C46" s="3"/>
+      <c r="D46" s="3"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="2">
         <v>44836</v>
       </c>
-      <c r="B47" s="5">
+      <c r="B47" s="3">
         <v>3</v>
       </c>
-      <c r="C47" s="5"/>
-      <c r="D47" s="5"/>
+      <c r="C47" s="3"/>
+      <c r="D47" s="3"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="4">
+      <c r="A49" s="2">
         <v>44837</v>
       </c>
-      <c r="B49" s="5">
+      <c r="B49" s="3">
         <v>2</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="5"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="4">
+      <c r="A50" s="2">
         <v>44838</v>
       </c>
-      <c r="B50" s="5">
+      <c r="B50" s="3">
         <v>9</v>
       </c>
-      <c r="C50" s="5"/>
-      <c r="D50" s="5"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="4">
+      <c r="A51" s="2">
         <v>44839</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="3">
         <v>5</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="5"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="4">
+      <c r="A52" s="2">
         <v>44840</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="3">
         <v>4</v>
       </c>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="3"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="4">
+      <c r="A53" s="2">
         <v>44841</v>
       </c>
-      <c r="B53" s="5">
+      <c r="B53" s="3">
         <v>5</v>
       </c>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5"/>
+      <c r="C53" s="3"/>
+      <c r="D53" s="3"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="4">
+      <c r="A54" s="2">
         <v>44842</v>
       </c>
-      <c r="B54" s="5">
+      <c r="B54" s="3">
         <v>10</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="5"/>
+      <c r="C54" s="3"/>
+      <c r="D54" s="3"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="4">
+      <c r="A55" s="2">
         <v>44843</v>
       </c>
-      <c r="B55" s="5">
+      <c r="B55" s="3">
         <v>10</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="5">
+      <c r="C55" s="3"/>
+      <c r="D55" s="3">
         <f>SUM(B49:B55) + 42</f>
         <v>87</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4">
+      <c r="A57" s="2">
         <v>44844</v>
       </c>
-      <c r="B57" s="5">
+      <c r="B57" s="3">
         <v>5</v>
       </c>
-      <c r="C57" s="5"/>
-      <c r="D57" s="5"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="4">
+      <c r="A58" s="2">
         <v>44845</v>
       </c>
-      <c r="B58" s="5">
+      <c r="B58" s="3">
         <v>9</v>
       </c>
-      <c r="C58" s="5"/>
-      <c r="D58" s="5"/>
+      <c r="C58" s="3"/>
+      <c r="D58" s="3"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="4">
+      <c r="A59" s="2">
         <v>44846</v>
       </c>
-      <c r="B59" s="5">
+      <c r="B59" s="3">
         <v>1</v>
       </c>
-      <c r="C59" s="5"/>
-      <c r="D59" s="5"/>
+      <c r="C59" s="3"/>
+      <c r="D59" s="3"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="4">
+      <c r="A60" s="2">
         <v>44847</v>
       </c>
-      <c r="B60" s="5">
+      <c r="B60" s="3">
         <v>1</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="5"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="4">
+      <c r="A61" s="2">
         <v>44848</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="3">
         <v>3</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="5"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="4">
+      <c r="A62" s="2">
         <v>44849</v>
       </c>
-      <c r="B62" s="5">
+      <c r="B62" s="3">
         <v>4</v>
       </c>
-      <c r="C62" s="5"/>
-      <c r="D62" s="5"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="4">
+      <c r="A63" s="2">
         <v>44850</v>
       </c>
-      <c r="B63" s="5">
+      <c r="B63" s="3">
         <v>4</v>
       </c>
-      <c r="C63" s="5"/>
-      <c r="D63" s="5">
+      <c r="C63" s="3"/>
+      <c r="D63" s="3">
         <f>SUM(B57:B63) + 42</f>
         <v>69</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="4">
+      <c r="A65" s="2">
         <v>44851</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="3">
         <v>1</v>
       </c>
-      <c r="C65" s="5"/>
-      <c r="D65" s="5"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="4">
+      <c r="A66" s="2">
         <v>44852</v>
       </c>
-      <c r="B66" s="5">
-        <v>0</v>
-      </c>
-      <c r="C66" s="5"/>
-      <c r="D66" s="5"/>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3"/>
+      <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="4">
+      <c r="A67" s="2">
         <v>44853</v>
       </c>
-      <c r="B67" s="5">
-        <v>0</v>
-      </c>
-      <c r="C67" s="5"/>
-      <c r="D67" s="5"/>
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3"/>
+      <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="4">
+      <c r="A68" s="2">
         <v>44854</v>
       </c>
-      <c r="B68" s="5">
-        <v>0</v>
-      </c>
-      <c r="C68" s="5"/>
-      <c r="D68" s="5"/>
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68" s="3"/>
+      <c r="D68" s="3"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="4">
+      <c r="A69" s="2">
         <v>44855</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="3">
         <v>4</v>
       </c>
-      <c r="C69" s="5"/>
-      <c r="D69" s="5"/>
+      <c r="C69" s="3"/>
+      <c r="D69" s="3"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="4">
+      <c r="A70" s="2">
         <v>44856</v>
       </c>
-      <c r="B70" s="5">
+      <c r="B70" s="3">
         <v>8</v>
       </c>
-      <c r="C70" s="5"/>
-      <c r="D70" s="5"/>
+      <c r="C70" s="3"/>
+      <c r="D70" s="3"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="4">
+      <c r="A71" s="2">
         <v>44857</v>
       </c>
-      <c r="B71" s="5">
+      <c r="B71" s="3">
         <v>12</v>
       </c>
-      <c r="C71" s="5"/>
-      <c r="D71" s="5">
+      <c r="C71" s="3"/>
+      <c r="D71" s="3">
         <f>SUM(B65:B71) + 42</f>
         <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="4">
+      <c r="A73" s="2">
         <v>44858</v>
       </c>
-      <c r="B73" s="5">
-        <v>0</v>
-      </c>
-      <c r="C73" s="5"/>
-      <c r="D73" s="5"/>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="4">
+      <c r="A74" s="2">
         <v>44859</v>
       </c>
-      <c r="B74" s="5">
+      <c r="B74" s="3">
         <v>2</v>
       </c>
-      <c r="C74" s="5"/>
-      <c r="D74" s="5"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="4">
+      <c r="A75" s="2">
         <v>44860</v>
       </c>
-      <c r="B75" s="5">
+      <c r="B75" s="3">
         <v>8</v>
       </c>
-      <c r="C75" s="5"/>
-      <c r="D75" s="5"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="4">
+      <c r="A76" s="2">
         <v>44861</v>
       </c>
-      <c r="B76" s="5">
+      <c r="B76" s="3">
         <v>11</v>
       </c>
-      <c r="C76" s="5"/>
-      <c r="D76" s="5"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="4">
+      <c r="A77" s="2">
         <v>44862</v>
       </c>
-      <c r="B77" s="5">
+      <c r="B77" s="3">
         <v>7</v>
       </c>
-      <c r="C77" s="5"/>
-      <c r="D77" s="5"/>
+      <c r="C77" s="3"/>
+      <c r="D77" s="3"/>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4">
+      <c r="A78" s="2">
         <v>44863</v>
       </c>
-      <c r="B78" s="5">
+      <c r="B78" s="3">
         <v>11</v>
       </c>
-      <c r="C78" s="5"/>
-      <c r="D78" s="5"/>
+      <c r="C78" s="3"/>
+      <c r="D78" s="3"/>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="4">
+      <c r="A79" s="2">
         <v>44864</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="3">
         <v>6</v>
       </c>
-      <c r="C79" s="5"/>
-      <c r="D79" s="5">
+      <c r="C79" s="3"/>
+      <c r="D79" s="3">
         <f>SUM(B73:B79) + 16</f>
         <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="4">
+      <c r="A81" s="2">
         <v>44865</v>
       </c>
-      <c r="B81" s="5">
+      <c r="B81" s="3">
         <v>8</v>
       </c>
-      <c r="C81" s="5"/>
-      <c r="D81" s="5"/>
+      <c r="C81" s="3"/>
+      <c r="D81" s="3"/>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="4">
+      <c r="A82" s="2">
         <v>44866</v>
       </c>
-      <c r="B82" s="5">
+      <c r="B82" s="3">
         <v>4</v>
       </c>
-      <c r="C82" s="5"/>
-      <c r="D82" s="5"/>
+      <c r="C82" s="3"/>
+      <c r="D82" s="3"/>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="4">
+      <c r="A83" s="2">
         <v>44867</v>
       </c>
-      <c r="B83" s="5">
+      <c r="B83" s="3">
         <v>7</v>
       </c>
-      <c r="C83" s="5"/>
-      <c r="D83" s="5"/>
+      <c r="C83" s="3"/>
+      <c r="D83" s="3"/>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="4">
+      <c r="A84" s="2">
         <v>44868</v>
       </c>
-      <c r="B84" s="5">
+      <c r="B84" s="3">
         <v>5</v>
       </c>
-      <c r="C84" s="5"/>
-      <c r="D84" s="5"/>
+      <c r="C84" s="3"/>
+      <c r="D84" s="3"/>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="4">
+      <c r="A85" s="2">
         <v>44869</v>
       </c>
-      <c r="B85" s="5">
+      <c r="B85" s="3">
         <v>4</v>
       </c>
-      <c r="C85" s="5"/>
-      <c r="D85" s="5"/>
+      <c r="C85" s="3"/>
+      <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="4">
+      <c r="A86" s="2">
         <v>44870</v>
       </c>
-      <c r="B86" s="5">
+      <c r="B86" s="3">
         <v>6</v>
       </c>
-      <c r="C86" s="5"/>
-      <c r="D86" s="5"/>
+      <c r="C86" s="3"/>
+      <c r="D86" s="3"/>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="4">
+      <c r="A87" s="2">
         <v>44871</v>
       </c>
-      <c r="B87" s="5">
+      <c r="B87" s="3">
         <v>3</v>
       </c>
-      <c r="C87" s="5"/>
-      <c r="D87" s="5"/>
+      <c r="C87" s="3"/>
+      <c r="D87" s="3"/>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="4">
+      <c r="A89" s="2">
         <v>44871</v>
       </c>
-      <c r="B89" s="5">
+      <c r="B89" s="3">
         <v>2</v>
       </c>
-      <c r="C89" s="5"/>
-      <c r="D89" s="5"/>
+      <c r="C89" s="3"/>
+      <c r="D89" s="3"/>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="4">
+      <c r="A90" s="2">
         <v>44872</v>
       </c>
-      <c r="B90" s="5">
+      <c r="B90" s="3">
         <v>4</v>
       </c>
-      <c r="C90" s="5"/>
-      <c r="D90" s="5"/>
+      <c r="C90" s="3"/>
+      <c r="D90" s="3"/>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="4">
+      <c r="A91" s="2">
         <v>44873</v>
       </c>
-      <c r="B91" s="5">
-        <v>0</v>
-      </c>
-      <c r="C91" s="5"/>
-      <c r="D91" s="5"/>
+      <c r="B91" s="3">
+        <v>0</v>
+      </c>
+      <c r="C91" s="3"/>
+      <c r="D91" s="3"/>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="A92" s="2">
         <v>44874</v>
       </c>
-      <c r="B92" s="5">
-        <v>0</v>
-      </c>
-      <c r="C92" s="5"/>
-      <c r="D92" s="5"/>
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92" s="3"/>
+      <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
+      <c r="A93" s="2">
         <v>44875</v>
       </c>
-      <c r="B93" s="5">
-        <v>0</v>
-      </c>
-      <c r="C93" s="5"/>
-      <c r="D93" s="5"/>
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3"/>
+      <c r="D93" s="3"/>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
+      <c r="A94" s="2">
         <v>44876</v>
       </c>
-      <c r="B94" s="5">
+      <c r="B94" s="3">
         <v>2</v>
       </c>
-      <c r="C94" s="5"/>
-      <c r="D94" s="5"/>
+      <c r="C94" s="3"/>
+      <c r="D94" s="3"/>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="A95" s="2">
         <v>44877</v>
       </c>
-      <c r="B95" s="5">
-        <v>0</v>
-      </c>
-      <c r="C95" s="5"/>
-      <c r="D95" s="5"/>
+      <c r="B95" s="3">
+        <v>0</v>
+      </c>
+      <c r="C95" s="3"/>
+      <c r="D95" s="3"/>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
+      <c r="A96" s="2">
         <v>44878</v>
       </c>
-      <c r="B96" s="5"/>
-      <c r="C96" s="5"/>
-      <c r="D96" s="5"/>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+      <c r="D96" s="3"/>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
+      <c r="A98" s="2">
         <v>44879</v>
       </c>
-      <c r="B98" s="5">
+      <c r="B98" s="3">
         <v>2</v>
       </c>
-      <c r="C98" s="5"/>
-      <c r="D98" s="5"/>
+      <c r="C98" s="3"/>
+      <c r="D98" s="3"/>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A99" s="4">
+      <c r="A99" s="2">
         <v>44880</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="3">
         <v>8</v>
       </c>
-      <c r="C99" s="5"/>
-      <c r="D99" s="5"/>
+      <c r="C99" s="3"/>
+      <c r="D99" s="3"/>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
+      <c r="A100" s="2">
         <v>44881</v>
       </c>
-      <c r="B100" s="5">
+      <c r="B100" s="3">
         <v>4</v>
       </c>
-      <c r="C100" s="5"/>
-      <c r="D100" s="5"/>
+      <c r="C100" s="3"/>
+      <c r="D100" s="3"/>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="A101" s="2">
         <v>44882</v>
       </c>
-      <c r="B101" s="5">
+      <c r="B101" s="3">
         <v>5</v>
       </c>
-      <c r="C101" s="5"/>
-      <c r="D101" s="5">
+      <c r="C101" s="3"/>
+      <c r="D101" s="3">
         <f>B101+10</f>
         <v>15</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="A102" s="2">
         <v>44883</v>
       </c>
-      <c r="B102" s="5">
+      <c r="B102" s="3">
         <v>7</v>
       </c>
-      <c r="C102" s="5"/>
-      <c r="D102" s="5">
+      <c r="C102" s="3"/>
+      <c r="D102" s="3">
         <f>B102+6</f>
         <v>13</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+      <c r="A103" s="2">
         <v>44884</v>
       </c>
-      <c r="B103" s="5">
+      <c r="B103" s="3">
         <v>8</v>
       </c>
-      <c r="C103" s="5"/>
-      <c r="D103" s="5"/>
+      <c r="C103" s="3"/>
+      <c r="D103" s="3"/>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="A104" s="2">
         <v>44885</v>
       </c>
-      <c r="B104" s="5">
+      <c r="B104" s="3">
         <v>4</v>
       </c>
-      <c r="C104" s="5"/>
-      <c r="D104" s="5">
+      <c r="C104" s="3"/>
+      <c r="D104" s="3">
         <f>SUM(B98:B104) + 42</f>
         <v>80</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
+      <c r="A106" s="2">
         <v>44886</v>
       </c>
-      <c r="B106" s="5">
+      <c r="B106" s="3">
         <v>5</v>
       </c>
-      <c r="C106" s="5"/>
-      <c r="D106" s="5"/>
+      <c r="C106" s="3"/>
+      <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
+      <c r="A107" s="2">
         <v>44887</v>
       </c>
-      <c r="B107" s="5">
-        <v>0</v>
-      </c>
-      <c r="C107" s="5"/>
-      <c r="D107" s="5"/>
+      <c r="B107" s="3">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3"/>
+      <c r="D107" s="3"/>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+      <c r="A108" s="2">
         <v>44888</v>
       </c>
-      <c r="B108" s="5">
+      <c r="B108" s="3">
         <v>5</v>
       </c>
-      <c r="C108" s="5"/>
-      <c r="D108" s="5"/>
+      <c r="C108" s="3"/>
+      <c r="D108" s="3"/>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
+      <c r="A109" s="2">
         <v>44889</v>
       </c>
-      <c r="B109" s="5">
-        <v>0</v>
-      </c>
-      <c r="C109" s="5"/>
-      <c r="D109" s="5"/>
+      <c r="B109" s="3">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3"/>
+      <c r="D109" s="3"/>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+      <c r="A110" s="2">
         <v>44890</v>
       </c>
-      <c r="B110" s="5">
+      <c r="B110" s="3">
         <v>5</v>
       </c>
-      <c r="C110" s="5"/>
-      <c r="D110" s="5"/>
+      <c r="C110" s="3"/>
+      <c r="D110" s="3"/>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="A111" s="2">
         <v>44891</v>
       </c>
-      <c r="B111" s="5">
+      <c r="B111" s="3">
         <v>12</v>
       </c>
-      <c r="C111" s="5"/>
-      <c r="D111" s="5"/>
+      <c r="C111" s="3"/>
+      <c r="D111" s="3"/>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+      <c r="A112" s="2">
         <v>44892</v>
       </c>
-      <c r="B112" s="5">
+      <c r="B112" s="3">
         <v>10</v>
       </c>
-      <c r="C112" s="5"/>
-      <c r="D112" s="5">
+      <c r="C112" s="3"/>
+      <c r="D112" s="3">
         <f>SUM(B106:B112) + 42</f>
         <v>79</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
+      <c r="A114" s="2">
         <v>44893</v>
       </c>
-      <c r="B114" s="5">
+      <c r="B114" s="3">
         <v>3</v>
       </c>
-      <c r="C114" s="5"/>
-      <c r="D114" s="5"/>
+      <c r="C114" s="3"/>
+      <c r="D114" s="3"/>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
+      <c r="A115" s="2">
         <v>44894</v>
       </c>
-      <c r="B115" s="5">
+      <c r="B115" s="3">
         <v>8</v>
       </c>
-      <c r="C115" s="5"/>
-      <c r="D115" s="5"/>
+      <c r="C115" s="3"/>
+      <c r="D115" s="3"/>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
+      <c r="A116" s="2">
         <v>44895</v>
       </c>
-      <c r="B116" s="5">
+      <c r="B116" s="3">
         <v>4</v>
       </c>
-      <c r="C116" s="5"/>
-      <c r="D116" s="5"/>
+      <c r="C116" s="3"/>
+      <c r="D116" s="3"/>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
+      <c r="A117" s="2">
         <v>44896</v>
       </c>
-      <c r="B117" s="5">
+      <c r="B117" s="3">
         <v>3</v>
       </c>
-      <c r="C117" s="5"/>
-      <c r="D117" s="5"/>
+      <c r="C117" s="3"/>
+      <c r="D117" s="3"/>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
+      <c r="A118" s="2">
         <v>44897</v>
       </c>
-      <c r="B118" s="5">
+      <c r="B118" s="3">
         <v>4</v>
       </c>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
+      <c r="C118" s="3"/>
+      <c r="D118" s="3"/>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
+      <c r="A119" s="2">
         <v>44898</v>
       </c>
-      <c r="B119" s="5">
+      <c r="B119" s="3">
         <v>8</v>
       </c>
-      <c r="C119" s="5"/>
-      <c r="D119" s="5"/>
+      <c r="C119" s="3"/>
+      <c r="D119" s="3"/>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
+      <c r="A120" s="2">
         <v>44899</v>
       </c>
-      <c r="B120" s="5">
+      <c r="B120" s="3">
         <v>13</v>
       </c>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5">
+      <c r="C120" s="3"/>
+      <c r="D120" s="3">
         <f>SUM(B114:B120) + 42</f>
         <v>85</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
+      <c r="A122" s="2">
         <v>44900</v>
       </c>
-      <c r="B122" s="5">
+      <c r="B122" s="3">
         <v>8</v>
       </c>
-      <c r="C122" s="5"/>
-      <c r="D122" s="5">
+      <c r="C122" s="3"/>
+      <c r="D122" s="3">
         <f>B122+10</f>
         <v>18</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
+      <c r="A123" s="2">
         <v>44901</v>
       </c>
-      <c r="B123" s="5">
+      <c r="B123" s="3">
         <v>6</v>
       </c>
-      <c r="C123" s="5"/>
-      <c r="D123" s="5"/>
+      <c r="C123" s="3"/>
+      <c r="D123" s="3"/>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A124" s="4">
+      <c r="A124" s="2">
         <v>44902</v>
       </c>
-      <c r="B124" s="5">
+      <c r="B124" s="3">
         <v>3</v>
       </c>
-      <c r="C124" s="5"/>
-      <c r="D124" s="5"/>
+      <c r="C124" s="3"/>
+      <c r="D124" s="3"/>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A125" s="4">
+      <c r="A125" s="2">
         <v>44903</v>
       </c>
-      <c r="B125" s="5">
+      <c r="B125" s="3">
         <v>10</v>
       </c>
-      <c r="C125" s="5"/>
-      <c r="D125" s="5"/>
+      <c r="C125" s="3"/>
+      <c r="D125" s="3"/>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A126" s="4">
+      <c r="A126" s="2">
         <v>44904</v>
       </c>
-      <c r="B126" s="5">
+      <c r="B126" s="3">
         <v>13</v>
       </c>
-      <c r="C126" s="5"/>
-      <c r="D126" s="5"/>
+      <c r="C126" s="3"/>
+      <c r="D126" s="3"/>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A127" s="4">
+      <c r="A127" s="2">
         <v>44905</v>
       </c>
-      <c r="B127" s="5">
+      <c r="B127" s="3">
         <v>10</v>
       </c>
-      <c r="C127" s="5"/>
-      <c r="D127" s="5"/>
+      <c r="C127" s="3"/>
+      <c r="D127" s="3"/>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A128" s="4">
+      <c r="A128" s="2">
         <v>44906</v>
       </c>
-      <c r="B128" s="5">
+      <c r="B128" s="3">
         <v>3</v>
       </c>
-      <c r="C128" s="5"/>
-      <c r="D128" s="5">
+      <c r="C128" s="3"/>
+      <c r="D128" s="3">
         <f>SUM(B122:B128) + 26</f>
         <v>79</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A130" s="4">
+      <c r="A130" s="2">
         <v>44921</v>
       </c>
-      <c r="B130" s="5">
-        <v>0</v>
-      </c>
-      <c r="C130" s="5"/>
-      <c r="D130" s="5"/>
+      <c r="B130" s="3">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3"/>
+      <c r="D130" s="3"/>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A131" s="4">
+      <c r="A131" s="2">
         <v>44922</v>
       </c>
-      <c r="B131" s="5">
+      <c r="B131" s="3">
         <v>5</v>
       </c>
-      <c r="C131" s="5"/>
-      <c r="D131" s="5"/>
+      <c r="C131" s="3"/>
+      <c r="D131" s="3"/>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A132" s="4">
+      <c r="A132" s="2">
         <v>44923</v>
       </c>
-      <c r="B132" s="5">
+      <c r="B132" s="3">
         <v>5</v>
       </c>
-      <c r="C132" s="5"/>
-      <c r="D132" s="5"/>
+      <c r="C132" s="3"/>
+      <c r="D132" s="3"/>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="4">
+      <c r="A133" s="2">
         <v>44924</v>
       </c>
-      <c r="B133" s="5">
-        <v>0</v>
-      </c>
-      <c r="C133" s="5"/>
-      <c r="D133" s="5"/>
+      <c r="B133" s="3">
+        <v>0</v>
+      </c>
+      <c r="C133" s="3"/>
+      <c r="D133" s="3"/>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A134" s="4">
+      <c r="A134" s="2">
         <v>44925</v>
       </c>
-      <c r="B134" s="5">
+      <c r="B134" s="3">
         <v>6</v>
       </c>
-      <c r="C134" s="5"/>
-      <c r="D134" s="5"/>
+      <c r="C134" s="3"/>
+      <c r="D134" s="3"/>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" s="4">
+      <c r="A135" s="2">
         <v>44926</v>
       </c>
-      <c r="B135" s="5">
+      <c r="B135" s="3">
         <v>8</v>
       </c>
-      <c r="C135" s="5"/>
-      <c r="D135" s="5"/>
+      <c r="C135" s="3"/>
+      <c r="D135" s="3"/>
     </row>
     <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A136" s="4">
+      <c r="A136" s="2">
         <v>44927</v>
       </c>
-      <c r="B136" s="5">
+      <c r="B136" s="3">
         <v>8</v>
       </c>
-      <c r="C136" s="5"/>
-      <c r="D136" s="5"/>
+      <c r="C136" s="3"/>
+      <c r="D136" s="3"/>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A138" s="4">
+      <c r="A138" s="2">
         <v>44928</v>
       </c>
-      <c r="B138" s="5">
+      <c r="B138" s="3">
         <v>8</v>
       </c>
-      <c r="C138" s="5"/>
-      <c r="D138" s="5"/>
+      <c r="C138" s="3"/>
+      <c r="D138" s="3"/>
     </row>
     <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="4">
+      <c r="A139" s="2">
         <v>44929</v>
       </c>
-      <c r="B139" s="5">
+      <c r="B139" s="3">
         <v>10</v>
       </c>
-      <c r="C139" s="5"/>
-      <c r="D139" s="5"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A140" s="4">
+      <c r="A140" s="2">
         <v>44930</v>
       </c>
-      <c r="B140" s="5">
+      <c r="B140" s="3">
         <v>10</v>
       </c>
-      <c r="C140" s="5"/>
-      <c r="D140" s="5"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" s="4">
+      <c r="A141" s="2">
         <v>44931</v>
       </c>
-      <c r="B141" s="5">
+      <c r="B141" s="3">
         <v>10</v>
       </c>
-      <c r="C141" s="5"/>
-      <c r="D141" s="5"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A142" s="4">
+      <c r="A142" s="2">
         <v>44932</v>
       </c>
-      <c r="B142" s="5">
+      <c r="B142" s="3">
         <v>10</v>
       </c>
-      <c r="C142" s="5"/>
-      <c r="D142" s="5"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A143" s="4">
+      <c r="A143" s="2">
         <v>44933</v>
       </c>
-      <c r="B143" s="5">
+      <c r="B143" s="3">
         <v>7</v>
       </c>
-      <c r="C143" s="5"/>
-      <c r="D143" s="5"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A144" s="4">
+      <c r="A144" s="2">
         <v>44934</v>
       </c>
-      <c r="B144" s="5">
+      <c r="B144" s="3">
         <v>5</v>
       </c>
-      <c r="C144" s="5"/>
-      <c r="D144" s="5"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A146" s="4">
+      <c r="A146" s="2">
         <v>44935</v>
       </c>
-      <c r="B146" s="5">
+      <c r="B146" s="3">
         <v>4</v>
       </c>
-      <c r="C146" s="5"/>
-      <c r="D146" s="5"/>
+      <c r="C146" s="3"/>
+      <c r="D146" s="3"/>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A147" s="4">
+      <c r="A147" s="2">
         <v>44936</v>
       </c>
-      <c r="B147" s="5">
+      <c r="B147" s="3">
         <v>7</v>
       </c>
-      <c r="C147" s="5"/>
-      <c r="D147" s="5"/>
+      <c r="C147" s="3"/>
+      <c r="D147" s="3"/>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A148" s="4">
+      <c r="A148" s="2">
         <v>44937</v>
       </c>
-      <c r="B148" s="5">
+      <c r="B148" s="3">
         <v>4</v>
       </c>
-      <c r="C148" s="5"/>
-      <c r="D148" s="5"/>
+      <c r="C148" s="3"/>
+      <c r="D148" s="3"/>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A149" s="4">
+      <c r="A149" s="2">
         <v>44938</v>
       </c>
-      <c r="B149" s="5">
+      <c r="B149" s="3">
         <v>3</v>
       </c>
-      <c r="C149" s="5"/>
-      <c r="D149" s="5"/>
+      <c r="C149" s="3"/>
+      <c r="D149" s="3"/>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A150" s="4">
+      <c r="A150" s="2">
         <v>44939</v>
       </c>
-      <c r="B150" s="5">
+      <c r="B150" s="3">
         <v>4</v>
       </c>
-      <c r="C150" s="5"/>
-      <c r="D150" s="5"/>
+      <c r="C150" s="3"/>
+      <c r="D150" s="3"/>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A151" s="4">
+      <c r="A151" s="2">
         <v>44940</v>
       </c>
-      <c r="B151" s="5">
+      <c r="B151" s="3">
         <v>8</v>
       </c>
-      <c r="C151" s="5"/>
-      <c r="D151" s="5"/>
+      <c r="C151" s="3"/>
+      <c r="D151" s="3"/>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A152" s="4">
+      <c r="A152" s="2">
         <v>44941</v>
       </c>
-      <c r="B152" s="5">
+      <c r="B152" s="3">
         <v>8</v>
       </c>
-      <c r="C152" s="5"/>
-      <c r="D152" s="5">
+      <c r="C152" s="3"/>
+      <c r="D152" s="3">
         <f>SUM(B146:B152) + 42</f>
         <v>80</v>
       </c>
     </row>
     <row r="154" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A154" s="4">
+      <c r="A154" s="2">
         <v>44942</v>
       </c>
-      <c r="B154" s="5">
+      <c r="B154" s="3">
         <v>3</v>
       </c>
-      <c r="C154" s="5"/>
-      <c r="D154" s="5"/>
+      <c r="C154" s="3"/>
+      <c r="D154" s="3"/>
     </row>
     <row r="155" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A155" s="4">
+      <c r="A155" s="2">
         <v>44943</v>
       </c>
-      <c r="B155" s="5">
+      <c r="B155" s="3">
         <v>4</v>
       </c>
-      <c r="C155" s="5"/>
-      <c r="D155" s="5"/>
+      <c r="C155" s="3"/>
+      <c r="D155" s="3"/>
     </row>
     <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="4">
+      <c r="A156" s="2">
         <v>44944</v>
       </c>
-      <c r="B156" s="5">
+      <c r="B156" s="3">
         <v>13</v>
       </c>
-      <c r="C156" s="5"/>
-      <c r="D156" s="5"/>
+      <c r="C156" s="3"/>
+      <c r="D156" s="3"/>
     </row>
     <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A157" s="4">
+      <c r="A157" s="2">
         <v>44945</v>
       </c>
-      <c r="B157" s="5">
+      <c r="B157" s="3">
         <v>5</v>
       </c>
-      <c r="C157" s="5"/>
-      <c r="D157" s="5"/>
+      <c r="C157" s="3"/>
+      <c r="D157" s="3"/>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" s="4">
+      <c r="A158" s="2">
         <v>44946</v>
       </c>
-      <c r="B158" s="5">
+      <c r="B158" s="3">
         <v>5</v>
       </c>
-      <c r="C158" s="5"/>
-      <c r="D158" s="5"/>
+      <c r="C158" s="3"/>
+      <c r="D158" s="3"/>
     </row>
     <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A159" s="4">
+      <c r="A159" s="2">
         <v>44947</v>
       </c>
-      <c r="B159" s="5">
+      <c r="B159" s="3">
         <v>12</v>
       </c>
-      <c r="C159" s="5"/>
-      <c r="D159" s="5"/>
+      <c r="C159" s="3"/>
+      <c r="D159" s="3"/>
     </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A160" s="4">
+      <c r="A160" s="2">
         <v>44948</v>
       </c>
-      <c r="B160" s="5">
+      <c r="B160" s="3">
         <v>11</v>
       </c>
-      <c r="C160" s="5"/>
-      <c r="D160" s="5">
+      <c r="C160" s="3"/>
+      <c r="D160" s="3">
         <f>SUM(B154:B160) + 32</f>
         <v>85</v>
       </c>
     </row>
     <row r="162" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A162" s="4">
+      <c r="A162" s="2">
         <v>44949</v>
       </c>
-      <c r="B162" s="5">
+      <c r="B162" s="3">
         <v>4</v>
       </c>
-      <c r="C162" s="5"/>
-      <c r="D162" s="5"/>
+      <c r="C162" s="3"/>
+      <c r="D162" s="3"/>
     </row>
     <row r="163" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A163" s="4">
+      <c r="A163" s="2">
         <v>44950</v>
       </c>
-      <c r="B163" s="5">
+      <c r="B163" s="3">
         <v>5</v>
       </c>
-      <c r="C163" s="5"/>
-      <c r="D163" s="5"/>
+      <c r="C163" s="3"/>
+      <c r="D163" s="3"/>
     </row>
     <row r="164" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A164" s="4">
+      <c r="A164" s="2">
         <v>44951</v>
       </c>
-      <c r="B164" s="5">
+      <c r="B164" s="3">
         <v>5</v>
       </c>
-      <c r="C164" s="5"/>
-      <c r="D164" s="5"/>
+      <c r="C164" s="3"/>
+      <c r="D164" s="3"/>
     </row>
     <row r="165" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A165" s="4">
+      <c r="A165" s="2">
         <v>44952</v>
       </c>
-      <c r="B165" s="5">
+      <c r="B165" s="3">
         <v>4</v>
       </c>
-      <c r="C165" s="5"/>
-      <c r="D165" s="5"/>
+      <c r="C165" s="3"/>
+      <c r="D165" s="3"/>
     </row>
     <row r="166" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A166" s="4">
+      <c r="A166" s="2">
         <v>44953</v>
       </c>
-      <c r="B166" s="5">
+      <c r="B166" s="3">
         <v>5</v>
       </c>
-      <c r="C166" s="5"/>
-      <c r="D166" s="5"/>
+      <c r="C166" s="3"/>
+      <c r="D166" s="3"/>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A167" s="4">
+      <c r="A167" s="2">
         <v>44954</v>
       </c>
-      <c r="B167" s="5">
+      <c r="B167" s="3">
         <v>4</v>
       </c>
-      <c r="C167" s="5"/>
-      <c r="D167" s="5"/>
+      <c r="C167" s="3"/>
+      <c r="D167" s="3"/>
     </row>
     <row r="168" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A168" s="4">
+      <c r="A168" s="2">
         <v>44955</v>
       </c>
-      <c r="B168" s="5">
+      <c r="B168" s="3">
         <v>7</v>
       </c>
-      <c r="C168" s="5"/>
-      <c r="D168" s="5"/>
+      <c r="C168" s="3"/>
+      <c r="D168" s="3"/>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A170" s="4">
+      <c r="A170" s="2">
         <v>44956</v>
       </c>
-      <c r="B170" s="5">
+      <c r="B170" s="3">
         <v>7</v>
       </c>
-      <c r="C170" s="5"/>
-      <c r="D170" s="5"/>
+      <c r="C170" s="3"/>
+      <c r="D170" s="3"/>
     </row>
     <row r="171" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A171" s="4">
+      <c r="A171" s="2">
         <v>44957</v>
       </c>
-      <c r="B171" s="5">
+      <c r="B171" s="3">
         <v>2</v>
       </c>
-      <c r="C171" s="5"/>
-      <c r="D171" s="5"/>
+      <c r="C171" s="3"/>
+      <c r="D171" s="3"/>
     </row>
     <row r="172" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A172" s="4">
+      <c r="A172" s="2">
         <v>44958</v>
       </c>
-      <c r="B172" s="5">
+      <c r="B172" s="3">
         <v>2</v>
       </c>
-      <c r="C172" s="5"/>
-      <c r="D172" s="5"/>
+      <c r="C172" s="3"/>
+      <c r="D172" s="3"/>
     </row>
     <row r="173" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A173" s="4">
+      <c r="A173" s="2">
         <v>44959</v>
       </c>
-      <c r="B173" s="5">
+      <c r="B173" s="3">
         <v>2</v>
       </c>
-      <c r="C173" s="5"/>
-      <c r="D173" s="5"/>
+      <c r="C173" s="3"/>
+      <c r="D173" s="3"/>
     </row>
     <row r="174" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A174" s="4">
+      <c r="A174" s="2">
         <v>44960</v>
       </c>
-      <c r="B174" s="5">
+      <c r="B174" s="3">
         <v>7</v>
       </c>
-      <c r="C174" s="5"/>
-      <c r="D174" s="5"/>
+      <c r="C174" s="3"/>
+      <c r="D174" s="3"/>
     </row>
     <row r="175" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A175" s="4">
+      <c r="A175" s="2">
         <v>44961</v>
       </c>
-      <c r="B175" s="5">
+      <c r="B175" s="3">
         <v>6</v>
       </c>
-      <c r="C175" s="5"/>
-      <c r="D175" s="5"/>
+      <c r="C175" s="3"/>
+      <c r="D175" s="3"/>
     </row>
     <row r="176" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A176" s="4">
+      <c r="A176" s="2">
         <v>44962</v>
       </c>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+      <c r="D176" s="2"/>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A178" s="4">
+      <c r="A178" s="2">
         <v>44963</v>
       </c>
-      <c r="B178" s="6">
+      <c r="B178" s="3">
         <v>3</v>
       </c>
-      <c r="C178" s="4"/>
-      <c r="D178" s="4"/>
+      <c r="C178" s="2"/>
+      <c r="D178" s="2"/>
     </row>
     <row r="179" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A179" s="4">
+      <c r="A179" s="2">
         <v>44964</v>
       </c>
-      <c r="B179" s="6">
+      <c r="B179" s="3">
         <v>2</v>
       </c>
-      <c r="C179" s="4"/>
-      <c r="D179" s="4"/>
+      <c r="C179" s="2"/>
+      <c r="D179" s="2"/>
     </row>
     <row r="180" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A180" s="4">
+      <c r="A180" s="2">
         <v>44965</v>
       </c>
-      <c r="B180" s="6">
-        <v>0</v>
-      </c>
-      <c r="C180" s="4"/>
-      <c r="D180" s="4"/>
+      <c r="B180" s="3">
+        <v>0</v>
+      </c>
+      <c r="C180" s="2"/>
+      <c r="D180" s="2"/>
     </row>
     <row r="181" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A181" s="4">
+      <c r="A181" s="2">
         <v>44966</v>
       </c>
-      <c r="B181" s="6">
-        <v>0</v>
-      </c>
-      <c r="C181" s="4"/>
-      <c r="D181" s="4"/>
+      <c r="B181" s="3">
+        <v>0</v>
+      </c>
+      <c r="C181" s="2"/>
+      <c r="D181" s="2"/>
     </row>
     <row r="182" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A182" s="4">
+      <c r="A182" s="2">
         <v>44967</v>
       </c>
-      <c r="B182" s="6">
-        <v>0</v>
-      </c>
-      <c r="C182" s="4"/>
-      <c r="D182" s="4"/>
+      <c r="B182" s="3">
+        <v>0</v>
+      </c>
+      <c r="C182" s="2"/>
+      <c r="D182" s="2"/>
     </row>
     <row r="183" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A183" s="4">
+      <c r="A183" s="2">
         <v>44968</v>
       </c>
-      <c r="B183" s="6">
+      <c r="B183" s="3">
         <v>3</v>
       </c>
-      <c r="C183" s="4"/>
-      <c r="D183" s="4"/>
+      <c r="C183" s="2"/>
+      <c r="D183" s="2"/>
     </row>
     <row r="184" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A184" s="4">
+      <c r="A184" s="2">
         <v>44969</v>
       </c>
-      <c r="B184" s="6">
+      <c r="B184" s="3">
         <v>8</v>
       </c>
-      <c r="C184" s="4"/>
-      <c r="D184" s="4"/>
+      <c r="C184" s="2"/>
+      <c r="D184" s="2"/>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A186" s="4">
+      <c r="A186" s="2">
         <v>44970</v>
       </c>
-      <c r="B186" s="6">
+      <c r="B186" s="3">
         <v>8</v>
       </c>
-      <c r="C186" s="4"/>
-      <c r="D186" s="4"/>
+      <c r="C186" s="2"/>
+      <c r="D186" s="2"/>
     </row>
     <row r="187" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A187" s="4">
+      <c r="A187" s="2">
         <v>44971</v>
       </c>
-      <c r="B187" s="6">
+      <c r="B187" s="3">
         <v>8</v>
       </c>
-      <c r="C187" s="4"/>
-      <c r="D187" s="4"/>
+      <c r="C187" s="2"/>
+      <c r="D187" s="2"/>
     </row>
     <row r="188" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A188" s="4">
+      <c r="A188" s="2">
         <v>44972</v>
       </c>
-      <c r="B188" s="6">
+      <c r="B188" s="3">
         <v>6</v>
       </c>
-      <c r="C188" s="4"/>
-      <c r="D188" s="4"/>
+      <c r="C188" s="2"/>
+      <c r="D188" s="2"/>
     </row>
     <row r="189" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A189" s="4">
+      <c r="A189" s="2">
         <v>44973</v>
       </c>
-      <c r="B189" s="6">
+      <c r="B189" s="3">
         <v>7</v>
       </c>
-      <c r="C189" s="4"/>
-      <c r="D189" s="4"/>
+      <c r="C189" s="2"/>
+      <c r="D189" s="2"/>
     </row>
     <row r="190" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A190" s="4">
+      <c r="A190" s="2">
         <v>44974</v>
       </c>
-      <c r="B190" s="6">
+      <c r="B190" s="3">
         <v>10</v>
       </c>
-      <c r="C190" s="4"/>
-      <c r="D190" s="4"/>
+      <c r="C190" s="2"/>
+      <c r="D190" s="2"/>
     </row>
     <row r="191" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A191" s="4">
+      <c r="A191" s="2">
         <v>44975</v>
       </c>
-      <c r="B191" s="6">
+      <c r="B191" s="3">
         <v>11</v>
       </c>
-      <c r="C191" s="4"/>
-      <c r="D191" s="4"/>
+      <c r="C191" s="2"/>
+      <c r="D191" s="2"/>
     </row>
     <row r="192" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A192" s="4">
+      <c r="A192" s="2">
         <v>44976</v>
       </c>
-      <c r="B192" s="6">
+      <c r="B192" s="3">
         <v>5</v>
       </c>
-      <c r="C192" s="4"/>
-      <c r="D192" s="4"/>
+      <c r="C192" s="2"/>
+      <c r="D192" s="2"/>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A194" s="4">
+      <c r="A194" s="2">
         <v>44977</v>
       </c>
-      <c r="B194" s="5">
+      <c r="B194" s="3">
         <v>1</v>
       </c>
-      <c r="C194" s="4"/>
-      <c r="D194" s="4"/>
+      <c r="C194" s="2"/>
+      <c r="D194" s="2"/>
     </row>
     <row r="195" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A195" s="4">
+      <c r="A195" s="2">
         <v>44978</v>
       </c>
-      <c r="B195" s="5">
+      <c r="B195" s="3">
         <v>5</v>
       </c>
-      <c r="C195" s="4"/>
-      <c r="D195" s="4"/>
+      <c r="C195" s="2"/>
+      <c r="D195" s="2"/>
     </row>
     <row r="196" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A196" s="4">
+      <c r="A196" s="2">
         <v>44979</v>
       </c>
-      <c r="B196" s="5">
+      <c r="B196" s="3">
         <v>2</v>
       </c>
-      <c r="C196" s="4"/>
-      <c r="D196" s="4"/>
+      <c r="C196" s="2"/>
+      <c r="D196" s="2"/>
     </row>
     <row r="197" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A197" s="4">
+      <c r="A197" s="2">
         <v>44980</v>
       </c>
-      <c r="B197" s="5">
+      <c r="B197" s="3">
         <v>5</v>
       </c>
-      <c r="C197" s="4"/>
-      <c r="D197" s="4"/>
+      <c r="C197" s="2"/>
+      <c r="D197" s="2"/>
     </row>
     <row r="198" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A198" s="4">
+      <c r="A198" s="2">
         <v>44981</v>
       </c>
-      <c r="B198" s="5">
+      <c r="B198" s="3">
         <v>3</v>
       </c>
-      <c r="C198" s="4"/>
-      <c r="D198" s="4"/>
+      <c r="C198" s="2"/>
+      <c r="D198" s="2"/>
     </row>
     <row r="199" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A199" s="4">
+      <c r="A199" s="2">
         <v>44982</v>
       </c>
-      <c r="B199" s="5">
+      <c r="B199" s="3">
         <v>10</v>
       </c>
-      <c r="C199" s="4"/>
-      <c r="D199" s="4"/>
+      <c r="C199" s="2"/>
+      <c r="D199" s="2"/>
     </row>
     <row r="200" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A200" s="4">
+      <c r="A200" s="2">
         <v>44983</v>
       </c>
-      <c r="B200" s="5">
+      <c r="B200" s="3">
         <v>5</v>
       </c>
-      <c r="C200" s="4"/>
-      <c r="D200" s="4"/>
+      <c r="C200" s="2"/>
+      <c r="D200" s="2"/>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A202" s="4">
+      <c r="A202" s="2">
         <v>44984</v>
       </c>
-      <c r="B202" s="5">
+      <c r="B202" s="3">
         <v>3</v>
       </c>
-      <c r="C202" s="5"/>
-      <c r="D202" s="5"/>
+      <c r="C202" s="3"/>
+      <c r="D202" s="3"/>
     </row>
     <row r="203" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A203" s="4">
+      <c r="A203" s="2">
         <v>44985</v>
       </c>
-      <c r="B203" s="5">
+      <c r="B203" s="3">
         <v>2</v>
       </c>
-      <c r="C203" s="5"/>
-      <c r="D203" s="5"/>
+      <c r="C203" s="3"/>
+      <c r="D203" s="3"/>
     </row>
     <row r="204" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A204" s="4">
+      <c r="A204" s="2">
         <v>44986</v>
       </c>
-      <c r="B204" s="5">
+      <c r="B204" s="3">
         <v>2</v>
       </c>
-      <c r="C204" s="5"/>
-      <c r="D204" s="5"/>
+      <c r="C204" s="3"/>
+      <c r="D204" s="3"/>
     </row>
     <row r="205" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A205" s="4">
+      <c r="A205" s="2">
         <v>44987</v>
       </c>
-      <c r="B205" s="5">
+      <c r="B205" s="3">
         <v>3</v>
       </c>
-      <c r="C205" s="5"/>
-      <c r="D205" s="5"/>
+      <c r="C205" s="3"/>
+      <c r="D205" s="3"/>
     </row>
     <row r="206" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A206" s="4">
+      <c r="A206" s="2">
         <v>44988</v>
       </c>
-      <c r="B206" s="5">
+      <c r="B206" s="3">
         <v>3</v>
       </c>
-      <c r="C206" s="5"/>
-      <c r="D206" s="5"/>
+      <c r="C206" s="3"/>
+      <c r="D206" s="3"/>
     </row>
     <row r="207" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A207" s="4">
+      <c r="A207" s="2">
         <v>44989</v>
       </c>
-      <c r="B207" s="5">
+      <c r="B207" s="3">
         <v>9</v>
       </c>
-      <c r="C207" s="5"/>
-      <c r="D207" s="5"/>
+      <c r="C207" s="3"/>
+      <c r="D207" s="3"/>
     </row>
     <row r="208" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A208" s="4">
+      <c r="A208" s="2">
         <v>44990</v>
       </c>
-      <c r="B208" s="5">
+      <c r="B208" s="3">
         <v>7</v>
       </c>
-      <c r="C208" s="5"/>
-      <c r="D208" s="5"/>
+      <c r="C208" s="3"/>
+      <c r="D208" s="3"/>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A210" s="4">
+      <c r="A210" s="2">
         <v>44991</v>
       </c>
-      <c r="B210" s="5">
+      <c r="B210" s="3">
         <v>2</v>
       </c>
-      <c r="C210" s="5"/>
-      <c r="D210" s="5"/>
+      <c r="C210" s="3"/>
+      <c r="D210" s="3"/>
     </row>
     <row r="211" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A211" s="4">
+      <c r="A211" s="2">
         <v>44992</v>
       </c>
-      <c r="B211" s="5">
+      <c r="B211" s="3">
         <v>2</v>
       </c>
-      <c r="C211" s="5"/>
-      <c r="D211" s="5"/>
+      <c r="C211" s="3"/>
+      <c r="D211" s="3"/>
     </row>
     <row r="212" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A212" s="4">
+      <c r="A212" s="2">
         <v>44993</v>
       </c>
-      <c r="B212" s="5">
+      <c r="B212" s="3">
         <v>5</v>
       </c>
-      <c r="C212" s="5"/>
-      <c r="D212" s="5"/>
+      <c r="C212" s="3"/>
+      <c r="D212" s="3"/>
     </row>
     <row r="213" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A213" s="4">
+      <c r="A213" s="2">
         <v>44994</v>
       </c>
-      <c r="B213" s="5">
+      <c r="B213" s="3">
         <v>3</v>
       </c>
-      <c r="C213" s="5"/>
-      <c r="D213" s="5"/>
+      <c r="C213" s="3"/>
+      <c r="D213" s="3"/>
     </row>
     <row r="214" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A214" s="4">
+      <c r="A214" s="2">
         <v>44995</v>
       </c>
-      <c r="B214" s="5">
+      <c r="B214" s="3">
         <v>2</v>
       </c>
-      <c r="C214" s="5"/>
-      <c r="D214" s="5"/>
+      <c r="C214" s="3"/>
+      <c r="D214" s="3"/>
     </row>
     <row r="215" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A215" s="4">
+      <c r="A215" s="2">
         <v>44996</v>
       </c>
-      <c r="B215" s="5">
+      <c r="B215" s="3">
         <v>8</v>
       </c>
-      <c r="C215" s="5"/>
-      <c r="D215" s="5"/>
+      <c r="C215" s="3"/>
+      <c r="D215" s="3"/>
     </row>
     <row r="216" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A216" s="4">
+      <c r="A216" s="2">
         <v>44997</v>
       </c>
-      <c r="B216" s="5">
+      <c r="B216" s="3">
         <v>7</v>
       </c>
-      <c r="C216" s="5"/>
-      <c r="D216" s="5"/>
+      <c r="C216" s="3"/>
+      <c r="D216" s="3"/>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A218" s="4">
+      <c r="A218" s="2">
         <v>44998</v>
       </c>
-      <c r="B218" s="5">
-        <v>0</v>
-      </c>
-      <c r="C218" s="5"/>
-      <c r="D218" s="5"/>
+      <c r="B218" s="3">
+        <v>0</v>
+      </c>
+      <c r="C218" s="3"/>
+      <c r="D218" s="3"/>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A219" s="4">
+      <c r="A219" s="2">
         <v>44999</v>
       </c>
-      <c r="B219" s="5">
-        <v>0</v>
-      </c>
-      <c r="C219" s="5"/>
-      <c r="D219" s="5"/>
+      <c r="B219" s="3">
+        <v>0</v>
+      </c>
+      <c r="C219" s="3"/>
+      <c r="D219" s="3"/>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A220" s="4">
+      <c r="A220" s="2">
         <v>45000</v>
       </c>
-      <c r="B220" s="5">
+      <c r="B220" s="3">
         <v>2</v>
       </c>
-      <c r="C220" s="5"/>
-      <c r="D220" s="5"/>
+      <c r="C220" s="3"/>
+      <c r="D220" s="3"/>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A221" s="4">
+      <c r="A221" s="2">
         <v>45001</v>
       </c>
-      <c r="B221" s="5">
+      <c r="B221" s="3">
         <v>1</v>
       </c>
-      <c r="C221" s="5"/>
-      <c r="D221" s="5"/>
+      <c r="C221" s="3"/>
+      <c r="D221" s="3"/>
     </row>
     <row r="222" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A222" s="4">
+      <c r="A222" s="2">
         <v>45002</v>
       </c>
-      <c r="B222" s="5">
+      <c r="B222" s="3">
         <v>3</v>
       </c>
-      <c r="C222" s="5"/>
-      <c r="D222" s="5"/>
+      <c r="C222" s="3"/>
+      <c r="D222" s="3"/>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A223" s="4">
+      <c r="A223" s="2">
         <v>45003</v>
       </c>
-      <c r="B223" s="5">
+      <c r="B223" s="3">
         <v>7</v>
       </c>
-      <c r="C223" s="5"/>
-      <c r="D223" s="5"/>
+      <c r="C223" s="3"/>
+      <c r="D223" s="3"/>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A224" s="4">
+      <c r="A224" s="2">
         <v>45004</v>
       </c>
-      <c r="B224" s="5">
+      <c r="B224" s="3">
         <v>2</v>
       </c>
-      <c r="C224" s="5"/>
-      <c r="D224" s="5"/>
+      <c r="C224" s="3"/>
+      <c r="D224" s="3"/>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A226" s="4">
+      <c r="A226" s="2">
         <v>45005</v>
       </c>
-      <c r="B226" s="5">
+      <c r="B226" s="3">
         <v>3</v>
       </c>
-      <c r="C226" s="5"/>
-      <c r="D226" s="5"/>
+      <c r="C226" s="3"/>
+      <c r="D226" s="3"/>
     </row>
     <row r="227" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A227" s="4">
+      <c r="A227" s="2">
         <v>45006</v>
       </c>
-      <c r="B227" s="5"/>
-      <c r="C227" s="5"/>
-      <c r="D227" s="5"/>
+      <c r="B227" s="3">
+        <v>9</v>
+      </c>
+      <c r="C227" s="3"/>
+      <c r="D227" s="3"/>
     </row>
     <row r="228" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A228" s="4">
+      <c r="A228" s="2">
         <v>45007</v>
       </c>
-      <c r="B228" s="5"/>
-      <c r="C228" s="5"/>
-      <c r="D228" s="5"/>
+      <c r="B228" s="3">
+        <v>9</v>
+      </c>
+      <c r="C228" s="3"/>
+      <c r="D228" s="3"/>
     </row>
     <row r="229" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A229" s="4">
+      <c r="A229" s="2">
         <v>45008</v>
       </c>
-      <c r="B229" s="5"/>
-      <c r="C229" s="5"/>
-      <c r="D229" s="5"/>
+      <c r="B229" s="3">
+        <v>4</v>
+      </c>
+      <c r="C229" s="3"/>
+      <c r="D229" s="3"/>
     </row>
     <row r="230" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A230" s="4">
+      <c r="A230" s="2">
         <v>45009</v>
       </c>
-      <c r="B230" s="5"/>
-      <c r="C230" s="5"/>
-      <c r="D230" s="5"/>
+      <c r="B230" s="3">
+        <v>9</v>
+      </c>
+      <c r="C230" s="3"/>
+      <c r="D230" s="3"/>
     </row>
     <row r="231" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A231" s="4">
+      <c r="A231" s="2">
         <v>45010</v>
       </c>
-      <c r="B231" s="5"/>
-      <c r="C231" s="5"/>
-      <c r="D231" s="5"/>
+      <c r="B231" s="3">
+        <v>9</v>
+      </c>
+      <c r="C231" s="3"/>
+      <c r="D231" s="3"/>
     </row>
     <row r="232" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A232" s="4">
+      <c r="A232" s="2">
         <v>45011</v>
       </c>
-      <c r="B232" s="5"/>
-      <c r="C232" s="5"/>
-      <c r="D232" s="5"/>
+      <c r="B232" s="3">
+        <v>9</v>
+      </c>
+      <c r="C232" s="3"/>
+      <c r="D232" s="3">
+        <f>SUM(B226:B232) + 42</f>
+        <v>94</v>
+      </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B234" s="5">
+      <c r="B234" s="3">
         <f>SUM(B2:B232)</f>
-        <v>928</v>
+        <v>977</v>
       </c>
       <c r="C234">
         <f>B234/25</f>
-        <v>37.119999999999997</v>
+        <v>39.08</v>
       </c>
       <c r="D234">
         <f>26*7</f>

</xml_diff>

<commit_message>
Added libraries to git
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B683E7CA-2E81-48AB-B2FE-AD8165AA6EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E87B3-8810-4C9D-B2C6-B55E81FAAB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20115" yWindow="1560" windowWidth="21060" windowHeight="13890" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="16890" yWindow="585" windowWidth="36135" windowHeight="15135" activeTab="1" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,22 +36,16 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>Tag</t>
-  </si>
-  <si>
-    <t>Working Routine</t>
-  </si>
-  <si>
-    <t>Mockup</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -63,6 +58,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF454545"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -91,11 +92,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -111,6 +113,2115 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:cat>
+            <c:strLit>
+              <c:ptCount val="32"/>
+              <c:pt idx="0">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>9</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>17</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>25</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>33</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>41</c:v>
+              </c:pt>
+              <c:pt idx="6">
+                <c:v>49</c:v>
+              </c:pt>
+              <c:pt idx="7">
+                <c:v>57</c:v>
+              </c:pt>
+              <c:pt idx="8">
+                <c:v>65</c:v>
+              </c:pt>
+              <c:pt idx="9">
+                <c:v>73</c:v>
+              </c:pt>
+              <c:pt idx="10">
+                <c:v>81</c:v>
+              </c:pt>
+              <c:pt idx="11">
+                <c:v>90</c:v>
+              </c:pt>
+              <c:pt idx="12">
+                <c:v>95</c:v>
+              </c:pt>
+              <c:pt idx="13">
+                <c:v>96</c:v>
+              </c:pt>
+              <c:pt idx="14">
+                <c:v>98</c:v>
+              </c:pt>
+              <c:pt idx="15">
+                <c:v>106</c:v>
+              </c:pt>
+              <c:pt idx="16">
+                <c:v>114</c:v>
+              </c:pt>
+              <c:pt idx="17">
+                <c:v>116</c:v>
+              </c:pt>
+              <c:pt idx="18">
+                <c:v>122</c:v>
+              </c:pt>
+              <c:pt idx="19">
+                <c:v>130</c:v>
+              </c:pt>
+              <c:pt idx="20">
+                <c:v>138</c:v>
+              </c:pt>
+              <c:pt idx="21">
+                <c:v>146</c:v>
+              </c:pt>
+              <c:pt idx="22">
+                <c:v>154</c:v>
+              </c:pt>
+              <c:pt idx="23">
+                <c:v>162</c:v>
+              </c:pt>
+              <c:pt idx="24">
+                <c:v>170</c:v>
+              </c:pt>
+              <c:pt idx="25">
+                <c:v>178</c:v>
+              </c:pt>
+              <c:pt idx="26">
+                <c:v>186</c:v>
+              </c:pt>
+              <c:pt idx="27">
+                <c:v>194</c:v>
+              </c:pt>
+              <c:pt idx="28">
+                <c:v>202</c:v>
+              </c:pt>
+              <c:pt idx="29">
+                <c:v>210</c:v>
+              </c:pt>
+              <c:pt idx="30">
+                <c:v>218</c:v>
+              </c:pt>
+              <c:pt idx="31">
+                <c:v>226</c:v>
+              </c:pt>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:autoCat val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:strLit>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Tabelle1!$D$7:$D$232</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>(Tabelle1!$D$7,Tabelle1!$D$15,Tabelle1!$D$23,Tabelle1!$D$31,Tabelle1!$D$39,Tabelle1!$D$47,Tabelle1!$D$55,Tabelle1!$D$63,Tabelle1!$D$71,Tabelle1!$D$79,Tabelle1!$D$87,Tabelle1!$D$96,Tabelle1!$D$101:$D$102,Tabelle1!$D$104,Tabelle1!$D$112,Tabelle1!$D$120,Tabelle1!$D$122,Tabelle1!$D$128,Tabelle1!$D$136,Tabelle1!$D$144,Tabelle1!$D$152,Tabelle1!$D$160,Tabelle1!$D$168,Tabelle1!$D$176,Tabelle1!$D$184,Tabelle1!$D$192,Tabelle1!$D$200,Tabelle1!$D$208,Tabelle1!$D$216,Tabelle1!$D$224,Tabelle1!$D$232)</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="32"/>
+                <c:pt idx="0">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>69</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>67</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>74</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>97</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6C89-4AC7-BDFF-82744B908010}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="378741840"/>
+        <c:axId val="378766800"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="378741840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378766800"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="378766800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="378741840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-DE"/>
+              <a:t>Hours/Week</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="de-DE"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle2!$E$1:$E$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>55</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2B97-46E1-A179-0978E890ED75}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="ctr"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="79"/>
+        <c:overlap val="100"/>
+        <c:axId val="1270733632"/>
+        <c:axId val="1270734880"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1270733632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Weeks</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1270734880"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1270734880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="1"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-DE"/>
+                  <a:t>Hours</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="1270733632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="298">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>173677</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>71499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>173677</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123206</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4A483B6-B09E-6665-684C-091A15A4472D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>285749</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Diagramm 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CF7C1A6C-6A12-3227-EB62-188E1446CAB5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -410,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:D234"/>
+  <dimension ref="A1:H234"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A214" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G228" sqref="G228"/>
+    <sheetView topLeftCell="A180" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection sqref="A1:D234"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,12 +2532,12 @@
     <col min="4" max="4" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44795</v>
       </c>
@@ -435,8 +2546,9 @@
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44796</v>
       </c>
@@ -444,11 +2556,9 @@
         <v>4</v>
       </c>
       <c r="C3" s="3"/>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44797</v>
       </c>
@@ -457,8 +2567,9 @@
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="H4" s="4"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44798</v>
       </c>
@@ -468,7 +2579,7 @@
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44799</v>
       </c>
@@ -476,11 +2587,9 @@
         <v>5</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44800</v>
       </c>
@@ -488,11 +2597,12 @@
         <v>11</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" s="3">
+        <f>SUM(B1:B7) + 42</f>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44801</v>
       </c>
@@ -502,7 +2612,7 @@
       <c r="C9" s="3"/>
       <c r="D9" s="3"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44802</v>
       </c>
@@ -512,7 +2622,7 @@
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44803</v>
       </c>
@@ -522,7 +2632,7 @@
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44805</v>
       </c>
@@ -532,7 +2642,7 @@
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44806</v>
       </c>
@@ -542,7 +2652,7 @@
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44807</v>
       </c>
@@ -552,7 +2662,7 @@
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44808</v>
       </c>
@@ -565,7 +2675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -709,7 +2819,10 @@
         <v>11</v>
       </c>
       <c r="C31" s="3"/>
-      <c r="D31" s="3"/>
+      <c r="D31" s="3">
+        <f>SUM(B25:B31) + 42</f>
+        <v>80</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
@@ -779,7 +2892,10 @@
         <v>0</v>
       </c>
       <c r="C39" s="3"/>
-      <c r="D39" s="3"/>
+      <c r="D39" s="3">
+        <f>SUM(B33:B39) + 42</f>
+        <v>47</v>
+      </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
@@ -849,7 +2965,10 @@
         <v>3</v>
       </c>
       <c r="C47" s="3"/>
-      <c r="D47" s="3"/>
+      <c r="D47" s="3">
+        <f>SUM(B41:B47) + 42</f>
+        <v>52</v>
+      </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
@@ -1211,7 +3330,10 @@
         <v>3</v>
       </c>
       <c r="C87" s="3"/>
-      <c r="D87" s="3"/>
+      <c r="D87" s="3">
+        <f>SUM(B81:B87) + 42</f>
+        <v>79</v>
+      </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
@@ -1289,7 +3411,10 @@
       </c>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
+      <c r="D96" s="3">
+        <f>SUM(B90:B96) + 42</f>
+        <v>48</v>
+      </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="2">
@@ -1328,11 +3453,11 @@
       <c r="B101" s="3">
         <v>5</v>
       </c>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3">
+      <c r="C101" s="3">
         <f>B101+10</f>
         <v>15</v>
       </c>
+      <c r="D101" s="3"/>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="2">
@@ -1341,11 +3466,11 @@
       <c r="B102" s="3">
         <v>7</v>
       </c>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3">
+      <c r="C102" s="3">
         <f>B102+6</f>
         <v>13</v>
       </c>
+      <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="2">
@@ -1523,11 +3648,11 @@
       <c r="B122" s="3">
         <v>8</v>
       </c>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3">
+      <c r="C122" s="3">
         <f>B122+10</f>
         <v>18</v>
       </c>
+      <c r="D122" s="3"/>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="2">
@@ -1660,7 +3785,10 @@
         <v>8</v>
       </c>
       <c r="C136" s="3"/>
-      <c r="D136" s="3"/>
+      <c r="D136" s="3">
+        <f>SUM(B130:B136) + 42</f>
+        <v>74</v>
+      </c>
     </row>
     <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="2">
@@ -1730,7 +3858,10 @@
         <v>5</v>
       </c>
       <c r="C144" s="3"/>
-      <c r="D144" s="3"/>
+      <c r="D144" s="3">
+        <f>SUM(B138:B144) + 42</f>
+        <v>102</v>
+      </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="2">
@@ -1946,7 +4077,10 @@
         <v>7</v>
       </c>
       <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
+      <c r="D168" s="3">
+        <f>SUM(B162:B168) + 42</f>
+        <v>76</v>
+      </c>
     </row>
     <row r="170" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A170" s="2">
@@ -2014,7 +4148,10 @@
       </c>
       <c r="B176" s="2"/>
       <c r="C176" s="2"/>
-      <c r="D176" s="2"/>
+      <c r="D176" s="3">
+        <f>SUM(B170:B176) + 42</f>
+        <v>68</v>
+      </c>
     </row>
     <row r="178" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A178" s="2">
@@ -2084,7 +4221,10 @@
         <v>8</v>
       </c>
       <c r="C184" s="2"/>
-      <c r="D184" s="2"/>
+      <c r="D184" s="3">
+        <f>SUM(B178:B184) + 42</f>
+        <v>58</v>
+      </c>
     </row>
     <row r="186" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A186" s="2">
@@ -2154,7 +4294,10 @@
         <v>5</v>
       </c>
       <c r="C192" s="2"/>
-      <c r="D192" s="2"/>
+      <c r="D192" s="3">
+        <f>SUM(B186:B192) + 42</f>
+        <v>97</v>
+      </c>
     </row>
     <row r="194" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A194" s="2">
@@ -2224,7 +4367,10 @@
         <v>5</v>
       </c>
       <c r="C200" s="2"/>
-      <c r="D200" s="2"/>
+      <c r="D200" s="3">
+        <f>SUM(B194:B200) + 42</f>
+        <v>73</v>
+      </c>
     </row>
     <row r="202" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A202" s="2">
@@ -2294,7 +4440,10 @@
         <v>7</v>
       </c>
       <c r="C208" s="3"/>
-      <c r="D208" s="3"/>
+      <c r="D208" s="3">
+        <f>SUM(B202:B208) + 42</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="210" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A210" s="2">
@@ -2364,7 +4513,10 @@
         <v>7</v>
       </c>
       <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
+      <c r="D216" s="3">
+        <f>SUM(B210:B216) + 42</f>
+        <v>71</v>
+      </c>
     </row>
     <row r="218" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A218" s="2">
@@ -2434,14 +4586,17 @@
         <v>2</v>
       </c>
       <c r="C224" s="3"/>
-      <c r="D224" s="3"/>
+      <c r="D224" s="3">
+        <f>SUM(B218:B224) + 42</f>
+        <v>57</v>
+      </c>
     </row>
     <row r="226" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A226" s="2">
         <v>45005</v>
       </c>
       <c r="B226" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C226" s="3"/>
       <c r="D226" s="3"/>
@@ -2501,22 +4656,22 @@
         <v>45011</v>
       </c>
       <c r="B232" s="3">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C232" s="3"/>
       <c r="D232" s="3">
         <f>SUM(B226:B232) + 42</f>
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B234" s="3">
         <f>SUM(B2:B232)</f>
-        <v>977</v>
+        <v>980</v>
       </c>
       <c r="C234">
         <f>B234/25</f>
-        <v>39.08</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="D234">
         <f>26*7</f>
@@ -2527,5 +4682,2108 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F5004A-DB6C-4584-B3FD-DC553DB69573}">
+  <dimension ref="A1:H234"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="3">
+        <f>SUM(B1:B7)</f>
+        <v>23</v>
+      </c>
+      <c r="E1">
+        <f>D1</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>44795</v>
+      </c>
+      <c r="B2" s="3">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3">
+        <f>SUM(B9:B15)</f>
+        <v>34</v>
+      </c>
+      <c r="E2">
+        <f>D2</f>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44796</v>
+      </c>
+      <c r="B3" s="3">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3">
+        <f>SUM(B17:B23)</f>
+        <v>39</v>
+      </c>
+      <c r="E3">
+        <f>D3</f>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44797</v>
+      </c>
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3">
+        <f>SUM(B25:B31) + 42</f>
+        <v>80</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="0">D4-42</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44798</v>
+      </c>
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3">
+        <f>SUM(B33:B39) + 42</f>
+        <v>47</v>
+      </c>
+      <c r="E5">
+        <f>D7-42</f>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44799</v>
+      </c>
+      <c r="B6" s="3">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3">
+        <f>SUM(B41:B47) + 42</f>
+        <v>52</v>
+      </c>
+      <c r="E6">
+        <f>D8-42</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44800</v>
+      </c>
+      <c r="B7" s="3">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3">
+        <f>SUM(B49:B55) + 42</f>
+        <v>87</v>
+      </c>
+      <c r="E7">
+        <f>D9-42</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D8" s="3">
+        <f>SUM(B57:B63) + 42</f>
+        <v>69</v>
+      </c>
+      <c r="E8">
+        <f>D10-42</f>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44801</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3">
+        <f>SUM(B65:B71) + 42</f>
+        <v>67</v>
+      </c>
+      <c r="E9">
+        <f>D11-42</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44802</v>
+      </c>
+      <c r="B10" s="3">
+        <v>4</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3">
+        <f>SUM(B73:B79) + 16</f>
+        <v>61</v>
+      </c>
+      <c r="E10">
+        <f>D12</f>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>44803</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3">
+        <f>SUM(B81:B87) + 42</f>
+        <v>79</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ref="E11:E21" si="1">D13-42</f>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>44805</v>
+      </c>
+      <c r="B12" s="3">
+        <v>3</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3">
+        <f>SUM(B90:B96) + 42</f>
+        <v>48</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>44806</v>
+      </c>
+      <c r="B13" s="3">
+        <v>4</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3">
+        <f>SUM(B98:B104) + 42</f>
+        <v>80</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>44807</v>
+      </c>
+      <c r="B14" s="3">
+        <v>4</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3">
+        <f>SUM(B106:B112) + 42</f>
+        <v>79</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>44808</v>
+      </c>
+      <c r="B15" s="3">
+        <v>15</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3">
+        <f>SUM(B114:B120) + 42</f>
+        <v>85</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="D16" s="3">
+        <f>SUM(B122:B128) + 26</f>
+        <v>79</v>
+      </c>
+      <c r="E16">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>44809</v>
+      </c>
+      <c r="B17" s="3">
+        <v>8</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3">
+        <f>SUM(B130:B136) + 42</f>
+        <v>74</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>44810</v>
+      </c>
+      <c r="B18" s="3">
+        <v>10</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3">
+        <f>SUM(B138:B144)</f>
+        <v>60</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>44811</v>
+      </c>
+      <c r="B19" s="3">
+        <v>12</v>
+      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3">
+        <f>SUM(B146:B152) + 42</f>
+        <v>80</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>44812</v>
+      </c>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3">
+        <f>SUM(B154:B160) + 32</f>
+        <v>85</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>44813</v>
+      </c>
+      <c r="B21" s="3">
+        <v>3</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3">
+        <f>SUM(B162:B168) + 42</f>
+        <v>76</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>44814</v>
+      </c>
+      <c r="B22" s="3">
+        <v>3</v>
+      </c>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3">
+        <f>SUM(B170:B176) + 42</f>
+        <v>68</v>
+      </c>
+      <c r="E22">
+        <f>D25-42</f>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>44815</v>
+      </c>
+      <c r="B23" s="3">
+        <v>0</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3">
+        <f>SUM(B178:B184) + 42</f>
+        <v>58</v>
+      </c>
+      <c r="E23">
+        <f>D26-42</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="D24" s="3">
+        <f>SUM(B186:B192)</f>
+        <v>55</v>
+      </c>
+      <c r="E24">
+        <f>D27-42</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>44816</v>
+      </c>
+      <c r="B25" s="3">
+        <v>0</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3">
+        <f>SUM(B194:B200) + 42</f>
+        <v>73</v>
+      </c>
+      <c r="E25">
+        <f>D28-42</f>
+        <v>15</v>
+      </c>
+      <c r="G25">
+        <f>B234</f>
+        <v>980</v>
+      </c>
+      <c r="H25">
+        <f>SUM(D2:D29)</f>
+        <v>1911</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>44817</v>
+      </c>
+      <c r="B26" s="3">
+        <v>7</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3">
+        <f>SUM(B202:B208) + 42</f>
+        <v>71</v>
+      </c>
+      <c r="E26">
+        <f>D29-42</f>
+        <v>55</v>
+      </c>
+      <c r="G26">
+        <f>C234</f>
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>44818</v>
+      </c>
+      <c r="B27" s="3">
+        <v>6</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3">
+        <f>SUM(B210:B216) + 42</f>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>44819</v>
+      </c>
+      <c r="B28" s="3">
+        <v>3</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3">
+        <f>SUM(B218:B224) + 42</f>
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>44820</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3">
+        <f>SUM(B226:B232) + 42</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>44821</v>
+      </c>
+      <c r="B30" s="3">
+        <v>9</v>
+      </c>
+      <c r="C30" s="3"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>44822</v>
+      </c>
+      <c r="B31" s="3">
+        <v>11</v>
+      </c>
+      <c r="C31" s="3"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>44823</v>
+      </c>
+      <c r="B33" s="3">
+        <v>0</v>
+      </c>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>44824</v>
+      </c>
+      <c r="B34" s="3">
+        <v>0</v>
+      </c>
+      <c r="C34" s="3"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>44825</v>
+      </c>
+      <c r="B35" s="3">
+        <v>2</v>
+      </c>
+      <c r="C35" s="3"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>44826</v>
+      </c>
+      <c r="B36" s="3">
+        <v>0</v>
+      </c>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>44827</v>
+      </c>
+      <c r="B37" s="3">
+        <v>0</v>
+      </c>
+      <c r="C37" s="3"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>44828</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>44829</v>
+      </c>
+      <c r="B39" s="3">
+        <v>0</v>
+      </c>
+      <c r="C39" s="3"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>44830</v>
+      </c>
+      <c r="B41" s="3">
+        <v>1</v>
+      </c>
+      <c r="C41" s="3"/>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>44831</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>44832</v>
+      </c>
+      <c r="B43" s="3">
+        <v>1</v>
+      </c>
+      <c r="C43" s="3"/>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>44833</v>
+      </c>
+      <c r="B44" s="3">
+        <v>1</v>
+      </c>
+      <c r="C44" s="3"/>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44834</v>
+      </c>
+      <c r="B45" s="3">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>44835</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="C46" s="3"/>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>44836</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3</v>
+      </c>
+      <c r="C47" s="3"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>44837</v>
+      </c>
+      <c r="B49" s="3">
+        <v>2</v>
+      </c>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>44838</v>
+      </c>
+      <c r="B50" s="3">
+        <v>9</v>
+      </c>
+      <c r="C50" s="3"/>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>44839</v>
+      </c>
+      <c r="B51" s="3">
+        <v>5</v>
+      </c>
+      <c r="C51" s="3"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>44840</v>
+      </c>
+      <c r="B52" s="3">
+        <v>4</v>
+      </c>
+      <c r="C52" s="3"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>44841</v>
+      </c>
+      <c r="B53" s="3">
+        <v>5</v>
+      </c>
+      <c r="C53" s="3"/>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>44842</v>
+      </c>
+      <c r="B54" s="3">
+        <v>10</v>
+      </c>
+      <c r="C54" s="3"/>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>44843</v>
+      </c>
+      <c r="B55" s="3">
+        <v>10</v>
+      </c>
+      <c r="C55" s="3"/>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>44844</v>
+      </c>
+      <c r="B57" s="3">
+        <v>5</v>
+      </c>
+      <c r="C57" s="3"/>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>44845</v>
+      </c>
+      <c r="B58" s="3">
+        <v>9</v>
+      </c>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>44846</v>
+      </c>
+      <c r="B59" s="3">
+        <v>1</v>
+      </c>
+      <c r="C59" s="3"/>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>44847</v>
+      </c>
+      <c r="B60" s="3">
+        <v>1</v>
+      </c>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>44848</v>
+      </c>
+      <c r="B61" s="3">
+        <v>3</v>
+      </c>
+      <c r="C61" s="3"/>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>44849</v>
+      </c>
+      <c r="B62" s="3">
+        <v>4</v>
+      </c>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>44850</v>
+      </c>
+      <c r="B63" s="3">
+        <v>4</v>
+      </c>
+      <c r="C63" s="3"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>44851</v>
+      </c>
+      <c r="B65" s="3">
+        <v>1</v>
+      </c>
+      <c r="C65" s="3"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>44852</v>
+      </c>
+      <c r="B66" s="3">
+        <v>0</v>
+      </c>
+      <c r="C66" s="3"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>44853</v>
+      </c>
+      <c r="B67" s="3">
+        <v>0</v>
+      </c>
+      <c r="C67" s="3"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>44854</v>
+      </c>
+      <c r="B68" s="3">
+        <v>0</v>
+      </c>
+      <c r="C68" s="3"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>44855</v>
+      </c>
+      <c r="B69" s="3">
+        <v>4</v>
+      </c>
+      <c r="C69" s="3"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>44856</v>
+      </c>
+      <c r="B70" s="3">
+        <v>8</v>
+      </c>
+      <c r="C70" s="3"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>44857</v>
+      </c>
+      <c r="B71" s="3">
+        <v>12</v>
+      </c>
+      <c r="C71" s="3"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>44858</v>
+      </c>
+      <c r="B73" s="3">
+        <v>0</v>
+      </c>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>44859</v>
+      </c>
+      <c r="B74" s="3">
+        <v>2</v>
+      </c>
+      <c r="C74" s="3"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>44860</v>
+      </c>
+      <c r="B75" s="3">
+        <v>8</v>
+      </c>
+      <c r="C75" s="3"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>44861</v>
+      </c>
+      <c r="B76" s="3">
+        <v>11</v>
+      </c>
+      <c r="C76" s="3"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>44862</v>
+      </c>
+      <c r="B77" s="3">
+        <v>7</v>
+      </c>
+      <c r="C77" s="3"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>44863</v>
+      </c>
+      <c r="B78" s="3">
+        <v>11</v>
+      </c>
+      <c r="C78" s="3"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>44864</v>
+      </c>
+      <c r="B79" s="3">
+        <v>6</v>
+      </c>
+      <c r="C79" s="3"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>44865</v>
+      </c>
+      <c r="B81" s="3">
+        <v>8</v>
+      </c>
+      <c r="C81" s="3"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>44866</v>
+      </c>
+      <c r="B82" s="3">
+        <v>4</v>
+      </c>
+      <c r="C82" s="3"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>44867</v>
+      </c>
+      <c r="B83" s="3">
+        <v>7</v>
+      </c>
+      <c r="C83" s="3"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>44868</v>
+      </c>
+      <c r="B84" s="3">
+        <v>5</v>
+      </c>
+      <c r="C84" s="3"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>44869</v>
+      </c>
+      <c r="B85" s="3">
+        <v>4</v>
+      </c>
+      <c r="C85" s="3"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>44870</v>
+      </c>
+      <c r="B86" s="3">
+        <v>6</v>
+      </c>
+      <c r="C86" s="3"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>44871</v>
+      </c>
+      <c r="B87" s="3">
+        <v>3</v>
+      </c>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>44871</v>
+      </c>
+      <c r="B89" s="3">
+        <v>2</v>
+      </c>
+      <c r="C89" s="3"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>44872</v>
+      </c>
+      <c r="B90" s="3">
+        <v>4</v>
+      </c>
+      <c r="C90" s="3"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>44873</v>
+      </c>
+      <c r="B91" s="3">
+        <v>0</v>
+      </c>
+      <c r="C91" s="3"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>44874</v>
+      </c>
+      <c r="B92" s="3">
+        <v>0</v>
+      </c>
+      <c r="C92" s="3"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="2">
+        <v>44875</v>
+      </c>
+      <c r="B93" s="3">
+        <v>0</v>
+      </c>
+      <c r="C93" s="3"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="2">
+        <v>44876</v>
+      </c>
+      <c r="B94" s="3">
+        <v>2</v>
+      </c>
+      <c r="C94" s="3"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="2">
+        <v>44877</v>
+      </c>
+      <c r="B95" s="3">
+        <v>0</v>
+      </c>
+      <c r="C95" s="3"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="2">
+        <v>44878</v>
+      </c>
+      <c r="B96" s="3"/>
+      <c r="C96" s="3"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="2">
+        <v>44879</v>
+      </c>
+      <c r="B98" s="3">
+        <v>2</v>
+      </c>
+      <c r="C98" s="3"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="2">
+        <v>44880</v>
+      </c>
+      <c r="B99" s="3">
+        <v>8</v>
+      </c>
+      <c r="C99" s="3"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="2">
+        <v>44881</v>
+      </c>
+      <c r="B100" s="3">
+        <v>4</v>
+      </c>
+      <c r="C100" s="3"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="2">
+        <v>44882</v>
+      </c>
+      <c r="B101" s="3">
+        <v>5</v>
+      </c>
+      <c r="C101" s="3">
+        <f>B101+10</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="2">
+        <v>44883</v>
+      </c>
+      <c r="B102" s="3">
+        <v>7</v>
+      </c>
+      <c r="C102" s="3">
+        <f>B102+6</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="2">
+        <v>44884</v>
+      </c>
+      <c r="B103" s="3">
+        <v>8</v>
+      </c>
+      <c r="C103" s="3"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="2">
+        <v>44885</v>
+      </c>
+      <c r="B104" s="3">
+        <v>4</v>
+      </c>
+      <c r="C104" s="3"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="2">
+        <v>44886</v>
+      </c>
+      <c r="B106" s="3">
+        <v>5</v>
+      </c>
+      <c r="C106" s="3"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="2">
+        <v>44887</v>
+      </c>
+      <c r="B107" s="3">
+        <v>0</v>
+      </c>
+      <c r="C107" s="3"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="2">
+        <v>44888</v>
+      </c>
+      <c r="B108" s="3">
+        <v>5</v>
+      </c>
+      <c r="C108" s="3"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="2">
+        <v>44889</v>
+      </c>
+      <c r="B109" s="3">
+        <v>0</v>
+      </c>
+      <c r="C109" s="3"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="2">
+        <v>44890</v>
+      </c>
+      <c r="B110" s="3">
+        <v>5</v>
+      </c>
+      <c r="C110" s="3"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="2">
+        <v>44891</v>
+      </c>
+      <c r="B111" s="3">
+        <v>12</v>
+      </c>
+      <c r="C111" s="3"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="2">
+        <v>44892</v>
+      </c>
+      <c r="B112" s="3">
+        <v>10</v>
+      </c>
+      <c r="C112" s="3"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="2">
+        <v>44893</v>
+      </c>
+      <c r="B114" s="3">
+        <v>3</v>
+      </c>
+      <c r="C114" s="3"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="2">
+        <v>44894</v>
+      </c>
+      <c r="B115" s="3">
+        <v>8</v>
+      </c>
+      <c r="C115" s="3"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="2">
+        <v>44895</v>
+      </c>
+      <c r="B116" s="3">
+        <v>4</v>
+      </c>
+      <c r="C116" s="3"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="2">
+        <v>44896</v>
+      </c>
+      <c r="B117" s="3">
+        <v>3</v>
+      </c>
+      <c r="C117" s="3"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="2">
+        <v>44897</v>
+      </c>
+      <c r="B118" s="3">
+        <v>4</v>
+      </c>
+      <c r="C118" s="3"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="2">
+        <v>44898</v>
+      </c>
+      <c r="B119" s="3">
+        <v>8</v>
+      </c>
+      <c r="C119" s="3"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="2">
+        <v>44899</v>
+      </c>
+      <c r="B120" s="3">
+        <v>13</v>
+      </c>
+      <c r="C120" s="3"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="2">
+        <v>44900</v>
+      </c>
+      <c r="B122" s="3">
+        <v>8</v>
+      </c>
+      <c r="C122" s="3">
+        <f>B122+10</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="2">
+        <v>44901</v>
+      </c>
+      <c r="B123" s="3">
+        <v>6</v>
+      </c>
+      <c r="C123" s="3"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="2">
+        <v>44902</v>
+      </c>
+      <c r="B124" s="3">
+        <v>3</v>
+      </c>
+      <c r="C124" s="3"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="2">
+        <v>44903</v>
+      </c>
+      <c r="B125" s="3">
+        <v>10</v>
+      </c>
+      <c r="C125" s="3"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="2">
+        <v>44904</v>
+      </c>
+      <c r="B126" s="3">
+        <v>13</v>
+      </c>
+      <c r="C126" s="3"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="2">
+        <v>44905</v>
+      </c>
+      <c r="B127" s="3">
+        <v>10</v>
+      </c>
+      <c r="C127" s="3"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="2">
+        <v>44906</v>
+      </c>
+      <c r="B128" s="3">
+        <v>3</v>
+      </c>
+      <c r="C128" s="3"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="2">
+        <v>44921</v>
+      </c>
+      <c r="B130" s="3">
+        <v>0</v>
+      </c>
+      <c r="C130" s="3"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="2">
+        <v>44922</v>
+      </c>
+      <c r="B131" s="3">
+        <v>5</v>
+      </c>
+      <c r="C131" s="3"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="2">
+        <v>44923</v>
+      </c>
+      <c r="B132" s="3">
+        <v>5</v>
+      </c>
+      <c r="C132" s="3"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="2">
+        <v>44924</v>
+      </c>
+      <c r="B133" s="3">
+        <v>0</v>
+      </c>
+      <c r="C133" s="3"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="2">
+        <v>44925</v>
+      </c>
+      <c r="B134" s="3">
+        <v>6</v>
+      </c>
+      <c r="C134" s="3"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="2">
+        <v>44926</v>
+      </c>
+      <c r="B135" s="3">
+        <v>8</v>
+      </c>
+      <c r="C135" s="3"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="2">
+        <v>44927</v>
+      </c>
+      <c r="B136" s="3">
+        <v>8</v>
+      </c>
+      <c r="C136" s="3"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="2">
+        <v>44928</v>
+      </c>
+      <c r="B138" s="3">
+        <v>8</v>
+      </c>
+      <c r="C138" s="3"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="2">
+        <v>44929</v>
+      </c>
+      <c r="B139" s="3">
+        <v>10</v>
+      </c>
+      <c r="C139" s="3"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="2">
+        <v>44930</v>
+      </c>
+      <c r="B140" s="3">
+        <v>10</v>
+      </c>
+      <c r="C140" s="3"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="2">
+        <v>44931</v>
+      </c>
+      <c r="B141" s="3">
+        <v>10</v>
+      </c>
+      <c r="C141" s="3"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="2">
+        <v>44932</v>
+      </c>
+      <c r="B142" s="3">
+        <v>10</v>
+      </c>
+      <c r="C142" s="3"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="2">
+        <v>44933</v>
+      </c>
+      <c r="B143" s="3">
+        <v>7</v>
+      </c>
+      <c r="C143" s="3"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="2">
+        <v>44934</v>
+      </c>
+      <c r="B144" s="3">
+        <v>5</v>
+      </c>
+      <c r="C144" s="3"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="2">
+        <v>44935</v>
+      </c>
+      <c r="B146" s="3">
+        <v>4</v>
+      </c>
+      <c r="C146" s="3"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="2">
+        <v>44936</v>
+      </c>
+      <c r="B147" s="3">
+        <v>7</v>
+      </c>
+      <c r="C147" s="3"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="2">
+        <v>44937</v>
+      </c>
+      <c r="B148" s="3">
+        <v>4</v>
+      </c>
+      <c r="C148" s="3"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="2">
+        <v>44938</v>
+      </c>
+      <c r="B149" s="3">
+        <v>3</v>
+      </c>
+      <c r="C149" s="3"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="2">
+        <v>44939</v>
+      </c>
+      <c r="B150" s="3">
+        <v>4</v>
+      </c>
+      <c r="C150" s="3"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="2">
+        <v>44940</v>
+      </c>
+      <c r="B151" s="3">
+        <v>8</v>
+      </c>
+      <c r="C151" s="3"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="2">
+        <v>44941</v>
+      </c>
+      <c r="B152" s="3">
+        <v>8</v>
+      </c>
+      <c r="C152" s="3"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="2">
+        <v>44942</v>
+      </c>
+      <c r="B154" s="3">
+        <v>3</v>
+      </c>
+      <c r="C154" s="3"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="2">
+        <v>44943</v>
+      </c>
+      <c r="B155" s="3">
+        <v>4</v>
+      </c>
+      <c r="C155" s="3"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="2">
+        <v>44944</v>
+      </c>
+      <c r="B156" s="3">
+        <v>13</v>
+      </c>
+      <c r="C156" s="3"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="2">
+        <v>44945</v>
+      </c>
+      <c r="B157" s="3">
+        <v>5</v>
+      </c>
+      <c r="C157" s="3"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="2">
+        <v>44946</v>
+      </c>
+      <c r="B158" s="3">
+        <v>5</v>
+      </c>
+      <c r="C158" s="3"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="2">
+        <v>44947</v>
+      </c>
+      <c r="B159" s="3">
+        <v>12</v>
+      </c>
+      <c r="C159" s="3"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="2">
+        <v>44948</v>
+      </c>
+      <c r="B160" s="3">
+        <v>11</v>
+      </c>
+      <c r="C160" s="3"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="2">
+        <v>44949</v>
+      </c>
+      <c r="B162" s="3">
+        <v>4</v>
+      </c>
+      <c r="C162" s="3"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="2">
+        <v>44950</v>
+      </c>
+      <c r="B163" s="3">
+        <v>5</v>
+      </c>
+      <c r="C163" s="3"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="2">
+        <v>44951</v>
+      </c>
+      <c r="B164" s="3">
+        <v>5</v>
+      </c>
+      <c r="C164" s="3"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="2">
+        <v>44952</v>
+      </c>
+      <c r="B165" s="3">
+        <v>4</v>
+      </c>
+      <c r="C165" s="3"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="2">
+        <v>44953</v>
+      </c>
+      <c r="B166" s="3">
+        <v>5</v>
+      </c>
+      <c r="C166" s="3"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="2">
+        <v>44954</v>
+      </c>
+      <c r="B167" s="3">
+        <v>4</v>
+      </c>
+      <c r="C167" s="3"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="2">
+        <v>44955</v>
+      </c>
+      <c r="B168" s="3">
+        <v>7</v>
+      </c>
+      <c r="C168" s="3"/>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="2">
+        <v>44956</v>
+      </c>
+      <c r="B170" s="3">
+        <v>7</v>
+      </c>
+      <c r="C170" s="3"/>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" s="2">
+        <v>44957</v>
+      </c>
+      <c r="B171" s="3">
+        <v>2</v>
+      </c>
+      <c r="C171" s="3"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="2">
+        <v>44958</v>
+      </c>
+      <c r="B172" s="3">
+        <v>2</v>
+      </c>
+      <c r="C172" s="3"/>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" s="2">
+        <v>44959</v>
+      </c>
+      <c r="B173" s="3">
+        <v>2</v>
+      </c>
+      <c r="C173" s="3"/>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="2">
+        <v>44960</v>
+      </c>
+      <c r="B174" s="3">
+        <v>7</v>
+      </c>
+      <c r="C174" s="3"/>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" s="2">
+        <v>44961</v>
+      </c>
+      <c r="B175" s="3">
+        <v>6</v>
+      </c>
+      <c r="C175" s="3"/>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="2">
+        <v>44962</v>
+      </c>
+      <c r="B176" s="2"/>
+      <c r="C176" s="2"/>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="2">
+        <v>44963</v>
+      </c>
+      <c r="B178" s="3">
+        <v>3</v>
+      </c>
+      <c r="C178" s="2"/>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" s="2">
+        <v>44964</v>
+      </c>
+      <c r="B179" s="3">
+        <v>2</v>
+      </c>
+      <c r="C179" s="2"/>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="2">
+        <v>44965</v>
+      </c>
+      <c r="B180" s="3">
+        <v>0</v>
+      </c>
+      <c r="C180" s="2"/>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" s="2">
+        <v>44966</v>
+      </c>
+      <c r="B181" s="3">
+        <v>0</v>
+      </c>
+      <c r="C181" s="2"/>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="2">
+        <v>44967</v>
+      </c>
+      <c r="B182" s="3">
+        <v>0</v>
+      </c>
+      <c r="C182" s="2"/>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" s="2">
+        <v>44968</v>
+      </c>
+      <c r="B183" s="3">
+        <v>3</v>
+      </c>
+      <c r="C183" s="2"/>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="2">
+        <v>44969</v>
+      </c>
+      <c r="B184" s="3">
+        <v>8</v>
+      </c>
+      <c r="C184" s="2"/>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="2">
+        <v>44970</v>
+      </c>
+      <c r="B186" s="3">
+        <v>8</v>
+      </c>
+      <c r="C186" s="2"/>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" s="2">
+        <v>44971</v>
+      </c>
+      <c r="B187" s="3">
+        <v>8</v>
+      </c>
+      <c r="C187" s="2"/>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="2">
+        <v>44972</v>
+      </c>
+      <c r="B188" s="3">
+        <v>6</v>
+      </c>
+      <c r="C188" s="2"/>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" s="2">
+        <v>44973</v>
+      </c>
+      <c r="B189" s="3">
+        <v>7</v>
+      </c>
+      <c r="C189" s="2"/>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="2">
+        <v>44974</v>
+      </c>
+      <c r="B190" s="3">
+        <v>10</v>
+      </c>
+      <c r="C190" s="2"/>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" s="2">
+        <v>44975</v>
+      </c>
+      <c r="B191" s="3">
+        <v>11</v>
+      </c>
+      <c r="C191" s="2"/>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="2">
+        <v>44976</v>
+      </c>
+      <c r="B192" s="3">
+        <v>5</v>
+      </c>
+      <c r="C192" s="2"/>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="2">
+        <v>44977</v>
+      </c>
+      <c r="B194" s="3">
+        <v>1</v>
+      </c>
+      <c r="C194" s="2"/>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" s="2">
+        <v>44978</v>
+      </c>
+      <c r="B195" s="3">
+        <v>5</v>
+      </c>
+      <c r="C195" s="2"/>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="2">
+        <v>44979</v>
+      </c>
+      <c r="B196" s="3">
+        <v>2</v>
+      </c>
+      <c r="C196" s="2"/>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" s="2">
+        <v>44980</v>
+      </c>
+      <c r="B197" s="3">
+        <v>5</v>
+      </c>
+      <c r="C197" s="2"/>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="2">
+        <v>44981</v>
+      </c>
+      <c r="B198" s="3">
+        <v>3</v>
+      </c>
+      <c r="C198" s="2"/>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" s="2">
+        <v>44982</v>
+      </c>
+      <c r="B199" s="3">
+        <v>10</v>
+      </c>
+      <c r="C199" s="2"/>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="2">
+        <v>44983</v>
+      </c>
+      <c r="B200" s="3">
+        <v>5</v>
+      </c>
+      <c r="C200" s="2"/>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="2">
+        <v>44984</v>
+      </c>
+      <c r="B202" s="3">
+        <v>3</v>
+      </c>
+      <c r="C202" s="3"/>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" s="2">
+        <v>44985</v>
+      </c>
+      <c r="B203" s="3">
+        <v>2</v>
+      </c>
+      <c r="C203" s="3"/>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="2">
+        <v>44986</v>
+      </c>
+      <c r="B204" s="3">
+        <v>2</v>
+      </c>
+      <c r="C204" s="3"/>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" s="2">
+        <v>44987</v>
+      </c>
+      <c r="B205" s="3">
+        <v>3</v>
+      </c>
+      <c r="C205" s="3"/>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="2">
+        <v>44988</v>
+      </c>
+      <c r="B206" s="3">
+        <v>3</v>
+      </c>
+      <c r="C206" s="3"/>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" s="2">
+        <v>44989</v>
+      </c>
+      <c r="B207" s="3">
+        <v>9</v>
+      </c>
+      <c r="C207" s="3"/>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="2">
+        <v>44990</v>
+      </c>
+      <c r="B208" s="3">
+        <v>7</v>
+      </c>
+      <c r="C208" s="3"/>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="2">
+        <v>44991</v>
+      </c>
+      <c r="B210" s="3">
+        <v>2</v>
+      </c>
+      <c r="C210" s="3"/>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" s="2">
+        <v>44992</v>
+      </c>
+      <c r="B211" s="3">
+        <v>2</v>
+      </c>
+      <c r="C211" s="3"/>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="2">
+        <v>44993</v>
+      </c>
+      <c r="B212" s="3">
+        <v>5</v>
+      </c>
+      <c r="C212" s="3"/>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" s="2">
+        <v>44994</v>
+      </c>
+      <c r="B213" s="3">
+        <v>3</v>
+      </c>
+      <c r="C213" s="3"/>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="2">
+        <v>44995</v>
+      </c>
+      <c r="B214" s="3">
+        <v>2</v>
+      </c>
+      <c r="C214" s="3"/>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" s="2">
+        <v>44996</v>
+      </c>
+      <c r="B215" s="3">
+        <v>8</v>
+      </c>
+      <c r="C215" s="3"/>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="2">
+        <v>44997</v>
+      </c>
+      <c r="B216" s="3">
+        <v>7</v>
+      </c>
+      <c r="C216" s="3"/>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="2">
+        <v>44998</v>
+      </c>
+      <c r="B218" s="3">
+        <v>0</v>
+      </c>
+      <c r="C218" s="3"/>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" s="2">
+        <v>44999</v>
+      </c>
+      <c r="B219" s="3">
+        <v>0</v>
+      </c>
+      <c r="C219" s="3"/>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="2">
+        <v>45000</v>
+      </c>
+      <c r="B220" s="3">
+        <v>2</v>
+      </c>
+      <c r="C220" s="3"/>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" s="2">
+        <v>45001</v>
+      </c>
+      <c r="B221" s="3">
+        <v>1</v>
+      </c>
+      <c r="C221" s="3"/>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="2">
+        <v>45002</v>
+      </c>
+      <c r="B222" s="3">
+        <v>3</v>
+      </c>
+      <c r="C222" s="3"/>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" s="2">
+        <v>45003</v>
+      </c>
+      <c r="B223" s="3">
+        <v>7</v>
+      </c>
+      <c r="C223" s="3"/>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="2">
+        <v>45004</v>
+      </c>
+      <c r="B224" s="3">
+        <v>2</v>
+      </c>
+      <c r="C224" s="3"/>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="2">
+        <v>45005</v>
+      </c>
+      <c r="B226" s="3">
+        <v>4</v>
+      </c>
+      <c r="C226" s="3"/>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" s="2">
+        <v>45006</v>
+      </c>
+      <c r="B227" s="3">
+        <v>9</v>
+      </c>
+      <c r="C227" s="3"/>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="2">
+        <v>45007</v>
+      </c>
+      <c r="B228" s="3">
+        <v>9</v>
+      </c>
+      <c r="C228" s="3"/>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" s="2">
+        <v>45008</v>
+      </c>
+      <c r="B229" s="3">
+        <v>4</v>
+      </c>
+      <c r="C229" s="3"/>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="2">
+        <v>45009</v>
+      </c>
+      <c r="B230" s="3">
+        <v>9</v>
+      </c>
+      <c r="C230" s="3"/>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" s="2">
+        <v>45010</v>
+      </c>
+      <c r="B231" s="3">
+        <v>9</v>
+      </c>
+      <c r="C231" s="3"/>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="2">
+        <v>45011</v>
+      </c>
+      <c r="B232" s="3">
+        <v>11</v>
+      </c>
+      <c r="C232" s="3"/>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B234" s="3">
+        <f>SUM(B2:B232)</f>
+        <v>980</v>
+      </c>
+      <c r="C234">
+        <f>B234/25</f>
+        <v>39.200000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added libs to embedded code
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{151E87B3-8810-4C9D-B2C6-B55E81FAAB91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2EFC91-12BD-43A7-B692-8444325BC4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="585" windowWidth="36135" windowHeight="15135" activeTab="1" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="16890" yWindow="585" windowWidth="36135" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2521,10 +2521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
-  <dimension ref="A1:H234"/>
+  <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView topLeftCell="A180" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:D234"/>
+    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G248" sqref="G248"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4665,15 +4665,257 @@
       </c>
     </row>
     <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A234" s="2">
+        <v>45012</v>
+      </c>
       <c r="B234" s="3">
-        <f>SUM(B2:B232)</f>
-        <v>980</v>
-      </c>
-      <c r="C234">
-        <f>B234/25</f>
-        <v>39.200000000000003</v>
-      </c>
-      <c r="D234">
+        <v>6</v>
+      </c>
+      <c r="C234" s="3"/>
+      <c r="D234" s="3"/>
+    </row>
+    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A235" s="2">
+        <v>45013</v>
+      </c>
+      <c r="B235" s="3"/>
+      <c r="C235" s="3"/>
+      <c r="D235" s="3"/>
+    </row>
+    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A236" s="2">
+        <v>45014</v>
+      </c>
+      <c r="B236" s="3"/>
+      <c r="C236" s="3"/>
+      <c r="D236" s="3"/>
+    </row>
+    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A237" s="2">
+        <v>45015</v>
+      </c>
+      <c r="B237" s="3"/>
+      <c r="C237" s="3"/>
+      <c r="D237" s="3"/>
+    </row>
+    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A238" s="2">
+        <v>45016</v>
+      </c>
+      <c r="B238" s="3">
+        <v>3</v>
+      </c>
+      <c r="C238" s="3"/>
+      <c r="D238" s="3"/>
+    </row>
+    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A239" s="2">
+        <v>45017</v>
+      </c>
+      <c r="B239" s="3">
+        <v>3</v>
+      </c>
+      <c r="C239" s="3"/>
+      <c r="D239" s="3"/>
+    </row>
+    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A240" s="2">
+        <v>45018</v>
+      </c>
+      <c r="B240" s="3">
+        <v>3</v>
+      </c>
+      <c r="C240" s="3"/>
+      <c r="D240" s="3"/>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A242" s="2">
+        <v>45019</v>
+      </c>
+      <c r="B242" s="3">
+        <v>3</v>
+      </c>
+      <c r="C242" s="3"/>
+      <c r="D242" s="3"/>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A243" s="2">
+        <v>45020</v>
+      </c>
+      <c r="B243" s="3"/>
+      <c r="C243" s="3"/>
+      <c r="D243" s="3"/>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A244" s="2">
+        <v>45021</v>
+      </c>
+      <c r="B244" s="3"/>
+      <c r="C244" s="3"/>
+      <c r="D244" s="3"/>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A245" s="2">
+        <v>45022</v>
+      </c>
+      <c r="B245" s="3"/>
+      <c r="C245" s="3"/>
+      <c r="D245" s="3"/>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A246" s="2">
+        <v>45023</v>
+      </c>
+      <c r="B246" s="3"/>
+      <c r="C246" s="3"/>
+      <c r="D246" s="3"/>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A247" s="2">
+        <v>45024</v>
+      </c>
+      <c r="B247" s="3"/>
+      <c r="C247" s="3"/>
+      <c r="D247" s="3"/>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A248" s="2">
+        <v>45025</v>
+      </c>
+      <c r="B248" s="3"/>
+      <c r="C248" s="3"/>
+      <c r="D248" s="3"/>
+    </row>
+    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A250" s="2">
+        <v>45026</v>
+      </c>
+      <c r="B250" s="3"/>
+      <c r="C250" s="3"/>
+      <c r="D250" s="3"/>
+    </row>
+    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A251" s="2">
+        <v>45027</v>
+      </c>
+      <c r="B251" s="3"/>
+      <c r="C251" s="3"/>
+      <c r="D251" s="3"/>
+    </row>
+    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A252" s="2">
+        <v>45028</v>
+      </c>
+      <c r="B252" s="3"/>
+      <c r="C252" s="3"/>
+      <c r="D252" s="3"/>
+    </row>
+    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A253" s="2">
+        <v>45029</v>
+      </c>
+      <c r="B253" s="3"/>
+      <c r="C253" s="3"/>
+      <c r="D253" s="3"/>
+    </row>
+    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A254" s="2">
+        <v>45030</v>
+      </c>
+      <c r="B254" s="3"/>
+      <c r="C254" s="3"/>
+      <c r="D254" s="3"/>
+    </row>
+    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A255" s="2">
+        <v>45031</v>
+      </c>
+      <c r="B255" s="3"/>
+      <c r="C255" s="3"/>
+      <c r="D255" s="3"/>
+    </row>
+    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A256" s="2">
+        <v>45032</v>
+      </c>
+      <c r="B256" s="3"/>
+      <c r="C256" s="3"/>
+      <c r="D256" s="3"/>
+    </row>
+    <row r="257" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A257" s="2">
+        <v>45033</v>
+      </c>
+      <c r="B257" s="3"/>
+      <c r="C257" s="3"/>
+      <c r="D257" s="3"/>
+    </row>
+    <row r="259" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A259" s="2">
+        <v>45034</v>
+      </c>
+      <c r="B259" s="3"/>
+      <c r="C259" s="3"/>
+      <c r="D259" s="3"/>
+    </row>
+    <row r="260" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A260" s="2">
+        <v>45035</v>
+      </c>
+      <c r="B260" s="3"/>
+      <c r="C260" s="3"/>
+      <c r="D260" s="3"/>
+    </row>
+    <row r="261" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A261" s="2">
+        <v>45036</v>
+      </c>
+      <c r="B261" s="3"/>
+      <c r="C261" s="3"/>
+      <c r="D261" s="3"/>
+    </row>
+    <row r="262" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A262" s="2">
+        <v>45037</v>
+      </c>
+      <c r="B262" s="3"/>
+      <c r="C262" s="3"/>
+      <c r="D262" s="3"/>
+    </row>
+    <row r="263" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A263" s="2">
+        <v>45038</v>
+      </c>
+      <c r="B263" s="3"/>
+      <c r="C263" s="3"/>
+      <c r="D263" s="3"/>
+    </row>
+    <row r="264" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A264" s="2">
+        <v>45039</v>
+      </c>
+      <c r="B264" s="3"/>
+      <c r="C264" s="3"/>
+      <c r="D264" s="3"/>
+    </row>
+    <row r="265" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A265" s="2">
+        <v>45040</v>
+      </c>
+      <c r="B265" s="3"/>
+      <c r="C265" s="3"/>
+      <c r="D265" s="3"/>
+    </row>
+    <row r="267" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B267" s="3">
+        <f>SUM(B2:B265)</f>
+        <v>998</v>
+      </c>
+      <c r="C267">
+        <f>B267/26</f>
+        <v>38.384615384615387</v>
+      </c>
+      <c r="D267">
         <f>26*7</f>
         <v>182</v>
       </c>
@@ -4690,7 +4932,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75F5004A-DB6C-4584-B3FD-DC553DB69573}">
   <dimension ref="A1:H234"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
working embedded wireless code
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2EFC91-12BD-43A7-B692-8444325BC4D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30E745F-F513-46B0-BAC8-B04DA45CEE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="585" windowWidth="36135" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="17700" yWindow="0" windowWidth="36135" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2523,8 +2523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A250" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G248" sqref="G248"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F240" sqref="F240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4678,7 +4678,9 @@
       <c r="A235" s="2">
         <v>45013</v>
       </c>
-      <c r="B235" s="3"/>
+      <c r="B235" s="3">
+        <v>0</v>
+      </c>
       <c r="C235" s="3"/>
       <c r="D235" s="3"/>
     </row>
@@ -4686,7 +4688,9 @@
       <c r="A236" s="2">
         <v>45014</v>
       </c>
-      <c r="B236" s="3"/>
+      <c r="B236" s="3">
+        <v>0</v>
+      </c>
       <c r="C236" s="3"/>
       <c r="D236" s="3"/>
     </row>
@@ -4694,7 +4698,9 @@
       <c r="A237" s="2">
         <v>45015</v>
       </c>
-      <c r="B237" s="3"/>
+      <c r="B237" s="3">
+        <v>0</v>
+      </c>
       <c r="C237" s="3"/>
       <c r="D237" s="3"/>
     </row>
@@ -4733,7 +4739,7 @@
         <v>45019</v>
       </c>
       <c r="B242" s="3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C242" s="3"/>
       <c r="D242" s="3"/>
@@ -4742,7 +4748,9 @@
       <c r="A243" s="2">
         <v>45020</v>
       </c>
-      <c r="B243" s="3"/>
+      <c r="B243" s="3">
+        <v>10</v>
+      </c>
       <c r="C243" s="3"/>
       <c r="D243" s="3"/>
     </row>
@@ -4750,7 +4758,9 @@
       <c r="A244" s="2">
         <v>45021</v>
       </c>
-      <c r="B244" s="3"/>
+      <c r="B244" s="3">
+        <v>7</v>
+      </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3"/>
     </row>
@@ -4909,15 +4919,15 @@
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B267" s="3">
         <f>SUM(B2:B265)</f>
-        <v>998</v>
+        <v>1018</v>
       </c>
       <c r="C267">
-        <f>B267/26</f>
-        <v>38.384615384615387</v>
+        <f>B267/27</f>
+        <v>37.703703703703702</v>
       </c>
       <c r="D267">
-        <f>26*7</f>
-        <v>182</v>
+        <f>27*7</f>
+        <v>189</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added Sleeptracker, Stepcounter, Health Algos.
</commit_message>
<xml_diff>
--- a/Data-Sheets/Mappe1.xlsx
+++ b/Data-Sheets/Mappe1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Project-Airframe\Data-Sheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Hardware\Project-Airframe\Data-Sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B30E745F-F513-46B0-BAC8-B04DA45CEE85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{075046AB-C35A-4BE1-9B48-8489E1FCFAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17700" yWindow="0" windowWidth="36135" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
+    <workbookView xWindow="5640" yWindow="810" windowWidth="21690" windowHeight="15135" xr2:uid="{546B7F45-972C-40FC-B9A3-D62BF07F438D}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -2523,7 +2523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B586C1-A708-43CB-9379-D0B63D1A81A1}">
   <dimension ref="A1:H267"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A259" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F240" sqref="F240"/>
     </sheetView>
   </sheetViews>
@@ -4759,7 +4759,7 @@
         <v>45021</v>
       </c>
       <c r="B244" s="3">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C244" s="3"/>
       <c r="D244" s="3"/>
@@ -4768,7 +4768,9 @@
       <c r="A245" s="2">
         <v>45022</v>
       </c>
-      <c r="B245" s="3"/>
+      <c r="B245" s="3">
+        <v>8</v>
+      </c>
       <c r="C245" s="3"/>
       <c r="D245" s="3"/>
     </row>
@@ -4776,7 +4778,9 @@
       <c r="A246" s="2">
         <v>45023</v>
       </c>
-      <c r="B246" s="3"/>
+      <c r="B246" s="3">
+        <v>9</v>
+      </c>
       <c r="C246" s="3"/>
       <c r="D246" s="3"/>
     </row>
@@ -4784,7 +4788,9 @@
       <c r="A247" s="2">
         <v>45024</v>
       </c>
-      <c r="B247" s="3"/>
+      <c r="B247" s="3">
+        <v>8</v>
+      </c>
       <c r="C247" s="3"/>
       <c r="D247" s="3"/>
     </row>
@@ -4794,7 +4800,10 @@
       </c>
       <c r="B248" s="3"/>
       <c r="C248" s="3"/>
-      <c r="D248" s="3"/>
+      <c r="D248" s="3">
+        <f>SUM(B242:B248)</f>
+        <v>53</v>
+      </c>
     </row>
     <row r="250" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A250" s="2">
@@ -4919,11 +4928,11 @@
     <row r="267" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B267" s="3">
         <f>SUM(B2:B265)</f>
-        <v>1018</v>
+        <v>1048</v>
       </c>
       <c r="C267">
         <f>B267/27</f>
-        <v>37.703703703703702</v>
+        <v>38.814814814814817</v>
       </c>
       <c r="D267">
         <f>27*7</f>

</xml_diff>